<commit_message>
LevelBuilder: fix bug with gameboard[5] appending the same r4c6 and s4d6 instead of r5d6 and s5d6, respectively.
</commit_message>
<xml_diff>
--- a/JSON/Levels16MoveList.xlsx
+++ b/JSON/Levels16MoveList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910A4899-2028-FE45-81C1-68878F1B7559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFEC3DC-2B04-9B4C-BD63-15406B8B3449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36020" yWindow="-2400" windowWidth="51180" windowHeight="24180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19515" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19560" uniqueCount="292">
   <si>
     <t>health</t>
   </si>
@@ -907,6 +907,12 @@
   <si>
     <t>s6d6</t>
   </si>
+  <si>
+    <t>D,D,R,R,D,L,D,L,D,U,U,L,L,U,R,U,R,R,D,L,D,R,R,D,D</t>
+  </si>
+  <si>
+    <t>R,D,D,D,D,D,R,R,R,U,L,L,U,R,R,U,L,L,L,U,U,R,D,U,R,U,R,R</t>
+  </si>
 </sst>
 </file>
 
@@ -1060,7 +1066,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1300,6 +1306,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1461,7 +1473,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1494,6 +1506,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1854,10 +1875,10 @@
   <dimension ref="A1:DC499"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="BZ362" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="B404" sqref="B404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -67704,15 +67725,17 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B403" s="8"/>
+      <c r="B403" s="8" t="s">
+        <v>290</v>
+      </c>
       <c r="C403" s="8"/>
       <c r="D403" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E403" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F403" s="10">
         <f t="shared" si="34"/>
@@ -67723,7 +67746,7 @@
         <v>401</v>
       </c>
       <c r="H403" s="11">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I403" s="11">
         <v>1</v>
@@ -67746,6 +67769,9 @@
       <c r="O403" t="s">
         <v>76</v>
       </c>
+      <c r="P403" t="s">
+        <v>76</v>
+      </c>
       <c r="Q403" s="12" t="s">
         <v>76</v>
       </c>
@@ -67764,7 +67790,9 @@
       <c r="V403" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W403" s="12"/>
+      <c r="W403" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X403" t="s">
         <v>76</v>
       </c>
@@ -67783,6 +67811,9 @@
       <c r="AC403" t="s">
         <v>76</v>
       </c>
+      <c r="AD403" t="s">
+        <v>76</v>
+      </c>
       <c r="AE403" s="12" t="s">
         <v>76</v>
       </c>
@@ -67801,7 +67832,9 @@
       <c r="AJ403" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK403" s="12"/>
+      <c r="AK403" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL403" t="s">
         <v>76</v>
       </c>
@@ -67820,6 +67853,9 @@
       <c r="AQ403" t="s">
         <v>76</v>
       </c>
+      <c r="AR403" t="s">
+        <v>76</v>
+      </c>
       <c r="AS403" s="12" t="s">
         <v>76</v>
       </c>
@@ -67836,93 +67872,130 @@
         <v>76</v>
       </c>
       <c r="AX403" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY403" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ403" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA403" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB403" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC403" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD403" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE403" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF403" t="s">
         <v>77</v>
       </c>
-      <c r="AY403" s="12"/>
       <c r="BG403" s="13"/>
-      <c r="BH403" s="13"/>
+      <c r="BH403" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="BI403" s="13" t="s">
         <v>79</v>
       </c>
       <c r="BJ403" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK403" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="BK403" s="13" t="s">
-        <v>78</v>
-      </c>
       <c r="BL403" s="13"/>
-      <c r="BM403" s="13"/>
-      <c r="BO403" t="s">
+      <c r="BM403" s="13" t="s">
         <v>78</v>
       </c>
       <c r="BP403" t="s">
         <v>79</v>
       </c>
-      <c r="BR403" t="s">
-        <v>78</v>
+      <c r="BQ403" t="s">
+        <v>79</v>
       </c>
       <c r="BS403" t="s">
-        <v>90</v>
-      </c>
-      <c r="BU403" s="13" t="s">
-        <v>82</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="BU403" s="13"/>
       <c r="BV403" s="13"/>
       <c r="BW403" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="BX403" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="BY403" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BZ403" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CA403" s="13"/>
-      <c r="CC403" t="s">
-        <v>79</v>
-      </c>
-      <c r="CD403" t="s">
-        <v>87</v>
+      <c r="BY403" s="13"/>
+      <c r="BZ403" s="13"/>
+      <c r="CA403" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="CB403" t="s">
+        <v>82</v>
       </c>
       <c r="CE403" t="s">
         <v>79</v>
       </c>
       <c r="CF403" t="s">
-        <v>90</v>
-      </c>
-      <c r="CI403" s="13" t="s">
-        <v>79</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="CG403" t="s">
+        <v>79</v>
+      </c>
+      <c r="CH403" t="s">
+        <v>79</v>
+      </c>
+      <c r="CI403" s="13"/>
       <c r="CJ403" s="13"/>
       <c r="CK403" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CL403" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CM403" s="13"/>
+        <v>87</v>
+      </c>
+      <c r="CM403" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="CN403" s="13" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="CO403" s="13"/>
+      <c r="CP403" t="s">
+        <v>78</v>
+      </c>
       <c r="CQ403" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CS403" t="s">
+        <v>78</v>
+      </c>
+      <c r="CT403" t="s">
+        <v>79</v>
+      </c>
+      <c r="CV403" t="s">
+        <v>78</v>
+      </c>
+      <c r="CW403" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CX403" s="13"/>
+      <c r="CY403" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CZ403" s="13"/>
+      <c r="DA403" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="CT403" t="s">
-        <v>79</v>
-      </c>
-      <c r="CW403" s="13"/>
-      <c r="CX403" s="13"/>
-      <c r="CY403" s="13"/>
-      <c r="CZ403" s="13"/>
-      <c r="DA403" s="13"/>
-      <c r="DB403" s="13"/>
+      <c r="DB403" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="DC403" s="13"/>
     </row>
     <row r="404" spans="1:107" x14ac:dyDescent="0.2">
@@ -67930,15 +68003,17 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B404" s="8"/>
+      <c r="B404" s="8" t="s">
+        <v>291</v>
+      </c>
       <c r="C404" s="8"/>
       <c r="D404" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E404" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F404" s="10">
         <f t="shared" si="34"/>
@@ -67949,7 +68024,7 @@
         <v>402</v>
       </c>
       <c r="H404" s="11">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I404" s="11">
         <v>1</v>
@@ -67970,6 +68045,9 @@
         <v>76</v>
       </c>
       <c r="O404" t="s">
+        <v>76</v>
+      </c>
+      <c r="P404" t="s">
         <v>77</v>
       </c>
       <c r="Q404" s="12" t="s">
@@ -67990,7 +68068,9 @@
       <c r="V404" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W404" s="12"/>
+      <c r="W404" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X404" t="s">
         <v>76</v>
       </c>
@@ -68009,6 +68089,9 @@
       <c r="AC404" t="s">
         <v>76</v>
       </c>
+      <c r="AD404" t="s">
+        <v>76</v>
+      </c>
       <c r="AE404" s="12" t="s">
         <v>76</v>
       </c>
@@ -68027,7 +68110,9 @@
       <c r="AJ404" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK404" s="12"/>
+      <c r="AK404" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL404" t="s">
         <v>76</v>
       </c>
@@ -68046,6 +68131,9 @@
       <c r="AQ404" t="s">
         <v>76</v>
       </c>
+      <c r="AR404" t="s">
+        <v>76</v>
+      </c>
       <c r="AS404" s="12" t="s">
         <v>76</v>
       </c>
@@ -68064,21 +68152,44 @@
       <c r="AX404" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AY404" s="12"/>
+      <c r="AY404" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ404" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA404" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB404" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC404" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD404" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE404" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF404" t="s">
+        <v>76</v>
+      </c>
       <c r="BG404" s="13"/>
-      <c r="BH404" s="13" t="s">
+      <c r="BH404" s="13"/>
+      <c r="BI404" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BI404" s="13" t="s">
+      <c r="BJ404" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="BJ404" s="13" t="s">
+      <c r="BK404" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="BK404" s="13"/>
       <c r="BL404" s="13"/>
       <c r="BM404" s="13"/>
-      <c r="BO404" t="s">
+      <c r="BN404" t="s">
         <v>79</v>
       </c>
       <c r="BP404" t="s">
@@ -68093,8 +68204,11 @@
       <c r="BS404" t="s">
         <v>79</v>
       </c>
+      <c r="BT404" t="s">
+        <v>79</v>
+      </c>
       <c r="BU404" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="BV404" s="13" t="s">
         <v>78</v>
@@ -68106,14 +68220,16 @@
         <v>78</v>
       </c>
       <c r="BY404" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="BZ404" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CA404" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="CA404" s="13"/>
       <c r="CB404" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CC404" t="s">
         <v>78</v>
@@ -68125,13 +68241,16 @@
         <v>78</v>
       </c>
       <c r="CF404" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CG404" t="s">
+        <v>79</v>
+      </c>
+      <c r="CH404" t="s">
         <v>87</v>
       </c>
       <c r="CI404" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CJ404" s="13" t="s">
         <v>78</v>
@@ -68143,14 +68262,16 @@
         <v>78</v>
       </c>
       <c r="CM404" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CN404" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CO404" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="CO404" s="13"/>
       <c r="CP404" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CQ404" t="s">
         <v>78</v>
@@ -68162,24 +68283,39 @@
         <v>78</v>
       </c>
       <c r="CT404" t="s">
-        <v>79</v>
-      </c>
-      <c r="CW404" s="13"/>
-      <c r="CX404" s="13"/>
-      <c r="CY404" s="13"/>
-      <c r="CZ404" s="13"/>
-      <c r="DA404" s="13"/>
-      <c r="DB404" s="13"/>
+        <v>78</v>
+      </c>
+      <c r="CU404" t="s">
+        <v>79</v>
+      </c>
+      <c r="CW404" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CX404" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CY404" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CZ404" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="DA404" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="DB404" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="DC404" s="13"/>
     </row>
     <row r="405" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A405" s="7">
+      <c r="A405" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B405" s="8"/>
-      <c r="C405" s="8"/>
-      <c r="D405" s="9">
+      <c r="B405" s="17"/>
+      <c r="C405" s="17"/>
+      <c r="D405" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -68417,13 +68553,13 @@
       <c r="DC405" s="13"/>
     </row>
     <row r="406" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A406" s="7">
+      <c r="A406" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B406" s="8"/>
-      <c r="C406" s="8"/>
-      <c r="D406" s="9">
+      <c r="B406" s="17"/>
+      <c r="C406" s="17"/>
+      <c r="D406" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -68648,13 +68784,13 @@
       <c r="DC406" s="13"/>
     </row>
     <row r="407" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A407" s="7">
+      <c r="A407" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B407" s="8"/>
-      <c r="C407" s="8"/>
-      <c r="D407" s="9">
+      <c r="B407" s="17"/>
+      <c r="C407" s="17"/>
+      <c r="D407" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -68893,13 +69029,13 @@
       <c r="DC407" s="13"/>
     </row>
     <row r="408" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A408" s="7">
+      <c r="A408" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B408" s="8"/>
-      <c r="C408" s="8"/>
-      <c r="D408" s="9">
+      <c r="B408" s="17"/>
+      <c r="C408" s="17"/>
+      <c r="D408" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -69147,13 +69283,13 @@
       <c r="DC408" s="13"/>
     </row>
     <row r="409" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A409" s="7">
+      <c r="A409" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B409" s="8"/>
-      <c r="C409" s="8"/>
-      <c r="D409" s="9">
+      <c r="B409" s="17"/>
+      <c r="C409" s="17"/>
+      <c r="D409" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -69387,13 +69523,13 @@
       <c r="DC409" s="13"/>
     </row>
     <row r="410" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A410" s="7">
+      <c r="A410" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B410" s="8"/>
-      <c r="C410" s="8"/>
-      <c r="D410" s="9">
+      <c r="B410" s="17"/>
+      <c r="C410" s="17"/>
+      <c r="D410" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -69631,13 +69767,13 @@
       <c r="DC410" s="13"/>
     </row>
     <row r="411" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A411" s="7">
+      <c r="A411" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B411" s="8"/>
-      <c r="C411" s="8"/>
-      <c r="D411" s="9">
+      <c r="B411" s="17"/>
+      <c r="C411" s="17"/>
+      <c r="D411" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -69860,13 +69996,13 @@
       <c r="DC411" s="13"/>
     </row>
     <row r="412" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A412" s="7">
+      <c r="A412" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B412" s="8"/>
-      <c r="C412" s="8"/>
-      <c r="D412" s="9">
+      <c r="B412" s="17"/>
+      <c r="C412" s="17"/>
+      <c r="D412" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -70114,13 +70250,13 @@
       <c r="DC412" s="13"/>
     </row>
     <row r="413" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A413" s="7">
+      <c r="A413" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B413" s="8"/>
-      <c r="C413" s="8"/>
-      <c r="D413" s="9">
+      <c r="B413" s="17"/>
+      <c r="C413" s="17"/>
+      <c r="D413" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -70368,13 +70504,13 @@
       <c r="DC413" s="13"/>
     </row>
     <row r="414" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A414" s="7">
+      <c r="A414" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B414" s="8"/>
-      <c r="C414" s="8"/>
-      <c r="D414" s="9">
+      <c r="B414" s="17"/>
+      <c r="C414" s="17"/>
+      <c r="D414" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -70608,13 +70744,13 @@
       <c r="DC414" s="13"/>
     </row>
     <row r="415" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A415" s="7">
+      <c r="A415" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B415" s="8"/>
-      <c r="C415" s="8"/>
-      <c r="D415" s="9">
+      <c r="B415" s="17"/>
+      <c r="C415" s="17"/>
+      <c r="D415" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -70854,13 +70990,13 @@
       <c r="DC415" s="13"/>
     </row>
     <row r="416" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A416" s="7">
+      <c r="A416" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B416" s="8"/>
-      <c r="C416" s="8"/>
-      <c r="D416" s="9">
+      <c r="B416" s="17"/>
+      <c r="C416" s="17"/>
+      <c r="D416" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -71085,13 +71221,13 @@
       <c r="DC416" s="13"/>
     </row>
     <row r="417" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A417" s="7">
+      <c r="A417" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B417" s="8"/>
-      <c r="C417" s="8"/>
-      <c r="D417" s="9">
+      <c r="B417" s="17"/>
+      <c r="C417" s="17"/>
+      <c r="D417" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -71331,13 +71467,13 @@
       <c r="DC417" s="13"/>
     </row>
     <row r="418" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A418" s="7">
+      <c r="A418" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B418" s="8"/>
-      <c r="C418" s="8"/>
-      <c r="D418" s="9">
+      <c r="B418" s="17"/>
+      <c r="C418" s="17"/>
+      <c r="D418" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -71585,13 +71721,13 @@
       <c r="DC418" s="13"/>
     </row>
     <row r="419" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A419" s="7">
+      <c r="A419" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B419" s="8"/>
-      <c r="C419" s="8"/>
-      <c r="D419" s="9">
+      <c r="B419" s="17"/>
+      <c r="C419" s="17"/>
+      <c r="D419" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -71824,13 +71960,13 @@
       <c r="DC419" s="13"/>
     </row>
     <row r="420" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A420" s="7">
+      <c r="A420" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B420" s="8"/>
-      <c r="C420" s="8"/>
-      <c r="D420" s="9">
+      <c r="B420" s="17"/>
+      <c r="C420" s="17"/>
+      <c r="D420" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -72073,13 +72209,13 @@
       <c r="DC420" s="13"/>
     </row>
     <row r="421" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A421" s="7">
+      <c r="A421" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B421" s="8"/>
-      <c r="C421" s="8"/>
-      <c r="D421" s="9">
+      <c r="B421" s="17"/>
+      <c r="C421" s="17"/>
+      <c r="D421" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -72287,13 +72423,13 @@
       <c r="DC421" s="13"/>
     </row>
     <row r="422" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A422" s="7">
+      <c r="A422" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B422" s="8"/>
-      <c r="C422" s="8"/>
-      <c r="D422" s="9">
+      <c r="B422" s="17"/>
+      <c r="C422" s="17"/>
+      <c r="D422" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -72527,13 +72663,13 @@
       <c r="DC422" s="13"/>
     </row>
     <row r="423" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A423" s="7">
+      <c r="A423" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B423" s="8"/>
-      <c r="C423" s="8"/>
-      <c r="D423" s="9">
+      <c r="B423" s="17"/>
+      <c r="C423" s="17"/>
+      <c r="D423" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -72764,13 +72900,13 @@
       <c r="DC423" s="13"/>
     </row>
     <row r="424" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A424" s="7">
+      <c r="A424" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B424" s="8"/>
-      <c r="C424" s="8"/>
-      <c r="D424" s="9">
+      <c r="B424" s="17"/>
+      <c r="C424" s="17"/>
+      <c r="D424" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -72979,13 +73115,13 @@
       <c r="DC424" s="13"/>
     </row>
     <row r="425" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A425" s="7">
+      <c r="A425" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B425" s="8"/>
-      <c r="C425" s="8"/>
-      <c r="D425" s="9">
+      <c r="B425" s="17"/>
+      <c r="C425" s="17"/>
+      <c r="D425" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -73233,13 +73369,13 @@
       <c r="DC425" s="13"/>
     </row>
     <row r="426" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A426" s="7">
+      <c r="A426" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B426" s="8"/>
-      <c r="C426" s="8"/>
-      <c r="D426" s="9">
+      <c r="B426" s="17"/>
+      <c r="C426" s="17"/>
+      <c r="D426" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -73485,13 +73621,13 @@
       <c r="DC426" s="13"/>
     </row>
     <row r="427" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A427" s="7">
+      <c r="A427" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B427" s="8"/>
-      <c r="C427" s="8"/>
-      <c r="D427" s="9">
+      <c r="B427" s="17"/>
+      <c r="C427" s="17"/>
+      <c r="D427" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -73712,13 +73848,13 @@
       <c r="DC427" s="13"/>
     </row>
     <row r="428" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A428" s="7">
+      <c r="A428" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B428" s="8"/>
-      <c r="C428" s="8"/>
-      <c r="D428" s="9">
+      <c r="B428" s="17"/>
+      <c r="C428" s="17"/>
+      <c r="D428" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -73919,13 +74055,13 @@
       <c r="DC428" s="13"/>
     </row>
     <row r="429" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A429" s="7">
+      <c r="A429" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B429" s="8"/>
-      <c r="C429" s="8"/>
-      <c r="D429" s="9">
+      <c r="B429" s="17"/>
+      <c r="C429" s="17"/>
+      <c r="D429" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -74145,13 +74281,13 @@
       <c r="DC429" s="13"/>
     </row>
     <row r="430" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A430" s="7">
+      <c r="A430" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B430" s="8"/>
-      <c r="C430" s="8"/>
-      <c r="D430" s="9">
+      <c r="B430" s="17"/>
+      <c r="C430" s="17"/>
+      <c r="D430" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -74389,13 +74525,13 @@
       <c r="DC430" s="13"/>
     </row>
     <row r="431" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A431" s="7">
+      <c r="A431" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B431" s="8"/>
-      <c r="C431" s="8"/>
-      <c r="D431" s="9">
+      <c r="B431" s="17"/>
+      <c r="C431" s="17"/>
+      <c r="D431" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -74619,13 +74755,13 @@
       <c r="DC431" s="13"/>
     </row>
     <row r="432" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A432" s="7">
+      <c r="A432" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B432" s="8"/>
-      <c r="C432" s="8"/>
-      <c r="D432" s="9">
+      <c r="B432" s="17"/>
+      <c r="C432" s="17"/>
+      <c r="D432" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -74867,13 +75003,13 @@
       <c r="DC432" s="13"/>
     </row>
     <row r="433" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A433" s="7">
+      <c r="A433" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B433" s="8"/>
-      <c r="C433" s="8"/>
-      <c r="D433" s="9">
+      <c r="B433" s="17"/>
+      <c r="C433" s="17"/>
+      <c r="D433" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -75115,13 +75251,13 @@
       <c r="DC433" s="13"/>
     </row>
     <row r="434" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A434" s="7">
+      <c r="A434" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B434" s="8"/>
-      <c r="C434" s="8"/>
-      <c r="D434" s="9">
+      <c r="B434" s="17"/>
+      <c r="C434" s="17"/>
+      <c r="D434" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -75351,13 +75487,13 @@
       <c r="DC434" s="13"/>
     </row>
     <row r="435" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A435" s="7">
+      <c r="A435" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B435" s="8"/>
-      <c r="C435" s="8"/>
-      <c r="D435" s="9">
+      <c r="B435" s="17"/>
+      <c r="C435" s="17"/>
+      <c r="D435" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -75581,13 +75717,13 @@
       <c r="DC435" s="13"/>
     </row>
     <row r="436" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A436" s="7">
+      <c r="A436" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B436" s="8"/>
-      <c r="C436" s="8"/>
-      <c r="D436" s="9">
+      <c r="B436" s="17"/>
+      <c r="C436" s="17"/>
+      <c r="D436" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -75821,13 +75957,13 @@
       <c r="DC436" s="13"/>
     </row>
     <row r="437" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A437" s="7">
+      <c r="A437" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B437" s="8"/>
-      <c r="C437" s="8"/>
-      <c r="D437" s="9">
+      <c r="B437" s="17"/>
+      <c r="C437" s="17"/>
+      <c r="D437" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -76066,13 +76202,13 @@
       <c r="DC437" s="13"/>
     </row>
     <row r="438" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A438" s="7">
+      <c r="A438" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B438" s="8"/>
-      <c r="C438" s="8"/>
-      <c r="D438" s="9">
+      <c r="B438" s="17"/>
+      <c r="C438" s="17"/>
+      <c r="D438" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -76287,13 +76423,13 @@
       <c r="DC438" s="13"/>
     </row>
     <row r="439" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A439" s="7">
+      <c r="A439" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B439" s="8"/>
-      <c r="C439" s="8"/>
-      <c r="D439" s="9">
+      <c r="B439" s="17"/>
+      <c r="C439" s="17"/>
+      <c r="D439" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -76510,13 +76646,13 @@
       <c r="DC439" s="13"/>
     </row>
     <row r="440" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A440" s="7">
+      <c r="A440" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B440" s="8"/>
-      <c r="C440" s="8"/>
-      <c r="D440" s="9">
+      <c r="B440" s="17"/>
+      <c r="C440" s="17"/>
+      <c r="D440" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -76751,13 +76887,13 @@
       <c r="DC440" s="13"/>
     </row>
     <row r="441" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A441" s="7">
+      <c r="A441" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B441" s="8"/>
-      <c r="C441" s="8"/>
-      <c r="D441" s="9">
+      <c r="B441" s="17"/>
+      <c r="C441" s="17"/>
+      <c r="D441" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -76980,13 +77116,13 @@
       <c r="DC441" s="13"/>
     </row>
     <row r="442" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A442" s="7">
+      <c r="A442" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B442" s="8"/>
-      <c r="C442" s="8"/>
-      <c r="D442" s="9">
+      <c r="B442" s="17"/>
+      <c r="C442" s="17"/>
+      <c r="D442" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -77234,13 +77370,13 @@
       <c r="DC442" s="13"/>
     </row>
     <row r="443" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A443" s="7">
+      <c r="A443" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B443" s="8"/>
-      <c r="C443" s="8"/>
-      <c r="D443" s="9">
+      <c r="B443" s="17"/>
+      <c r="C443" s="17"/>
+      <c r="D443" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -77449,13 +77585,13 @@
       <c r="DC443" s="13"/>
     </row>
     <row r="444" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A444" s="7">
+      <c r="A444" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B444" s="8"/>
-      <c r="C444" s="8"/>
-      <c r="D444" s="9">
+      <c r="B444" s="17"/>
+      <c r="C444" s="17"/>
+      <c r="D444" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -77673,13 +77809,13 @@
       <c r="DC444" s="13"/>
     </row>
     <row r="445" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A445" s="7">
+      <c r="A445" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B445" s="8"/>
-      <c r="C445" s="8"/>
-      <c r="D445" s="9">
+      <c r="B445" s="17"/>
+      <c r="C445" s="17"/>
+      <c r="D445" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -77923,13 +78059,13 @@
       <c r="DC445" s="13"/>
     </row>
     <row r="446" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A446" s="7">
+      <c r="A446" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B446" s="8"/>
-      <c r="C446" s="8"/>
-      <c r="D446" s="9">
+      <c r="B446" s="17"/>
+      <c r="C446" s="17"/>
+      <c r="D446" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -78161,13 +78297,13 @@
       <c r="DC446" s="13"/>
     </row>
     <row r="447" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A447" s="7">
+      <c r="A447" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B447" s="8"/>
-      <c r="C447" s="8"/>
-      <c r="D447" s="9">
+      <c r="B447" s="17"/>
+      <c r="C447" s="17"/>
+      <c r="D447" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -78385,13 +78521,13 @@
       <c r="DC447" s="13"/>
     </row>
     <row r="448" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A448" s="7">
+      <c r="A448" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B448" s="8"/>
-      <c r="C448" s="8"/>
-      <c r="D448" s="9">
+      <c r="B448" s="17"/>
+      <c r="C448" s="17"/>
+      <c r="D448" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -78591,13 +78727,13 @@
       <c r="DC448" s="13"/>
     </row>
     <row r="449" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A449" s="7">
+      <c r="A449" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B449" s="8"/>
-      <c r="C449" s="8"/>
-      <c r="D449" s="9">
+      <c r="B449" s="17"/>
+      <c r="C449" s="17"/>
+      <c r="D449" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -78830,13 +78966,13 @@
       <c r="DC449" s="13"/>
     </row>
     <row r="450" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A450" s="7">
+      <c r="A450" s="16">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B450" s="8"/>
-      <c r="C450" s="8"/>
-      <c r="D450" s="9">
+      <c r="B450" s="17"/>
+      <c r="C450" s="17"/>
+      <c r="D450" s="18">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -79052,13 +79188,13 @@
       <c r="DC450" s="13"/>
     </row>
     <row r="451" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A451" s="7">
+      <c r="A451" s="16">
         <f t="shared" ref="A451:A497" si="36">COUNTA(J451:O451)</f>
         <v>6</v>
       </c>
-      <c r="B451" s="8"/>
-      <c r="C451" s="8"/>
-      <c r="D451" s="9">
+      <c r="B451" s="17"/>
+      <c r="C451" s="17"/>
+      <c r="D451" s="18">
         <f t="shared" ref="D451:D497" si="37">LEN(B451)-LEN(SUBSTITUTE(B451,",",""))+1</f>
         <v>1</v>
       </c>
@@ -79261,13 +79397,13 @@
       <c r="DC451" s="13"/>
     </row>
     <row r="452" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A452" s="7">
+      <c r="A452" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B452" s="8"/>
-      <c r="C452" s="8"/>
-      <c r="D452" s="9">
+      <c r="B452" s="17"/>
+      <c r="C452" s="17"/>
+      <c r="D452" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -79475,13 +79611,13 @@
       <c r="DC452" s="13"/>
     </row>
     <row r="453" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A453" s="7">
+      <c r="A453" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B453" s="8"/>
-      <c r="C453" s="8"/>
-      <c r="D453" s="9">
+      <c r="B453" s="17"/>
+      <c r="C453" s="17"/>
+      <c r="D453" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -79695,13 +79831,13 @@
       <c r="DC453" s="13"/>
     </row>
     <row r="454" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A454" s="7">
+      <c r="A454" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B454" s="8"/>
-      <c r="C454" s="8"/>
-      <c r="D454" s="9">
+      <c r="B454" s="17"/>
+      <c r="C454" s="17"/>
+      <c r="D454" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -79924,13 +80060,13 @@
       <c r="DC454" s="13"/>
     </row>
     <row r="455" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A455" s="7">
+      <c r="A455" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B455" s="8"/>
-      <c r="C455" s="8"/>
-      <c r="D455" s="9">
+      <c r="B455" s="17"/>
+      <c r="C455" s="17"/>
+      <c r="D455" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -80151,13 +80287,13 @@
       <c r="DC455" s="13"/>
     </row>
     <row r="456" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A456" s="7">
+      <c r="A456" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B456" s="8"/>
-      <c r="C456" s="8"/>
-      <c r="D456" s="9">
+      <c r="B456" s="17"/>
+      <c r="C456" s="17"/>
+      <c r="D456" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -80375,13 +80511,13 @@
       <c r="DC456" s="13"/>
     </row>
     <row r="457" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A457" s="7">
+      <c r="A457" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B457" s="8"/>
-      <c r="C457" s="8"/>
-      <c r="D457" s="9">
+      <c r="B457" s="17"/>
+      <c r="C457" s="17"/>
+      <c r="D457" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -80602,13 +80738,13 @@
       <c r="DC457" s="13"/>
     </row>
     <row r="458" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A458" s="7">
+      <c r="A458" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B458" s="8"/>
-      <c r="C458" s="8"/>
-      <c r="D458" s="9">
+      <c r="B458" s="17"/>
+      <c r="C458" s="17"/>
+      <c r="D458" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -80808,13 +80944,13 @@
       <c r="DC458" s="13"/>
     </row>
     <row r="459" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A459" s="7">
+      <c r="A459" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B459" s="8"/>
-      <c r="C459" s="8"/>
-      <c r="D459" s="9">
+      <c r="B459" s="17"/>
+      <c r="C459" s="17"/>
+      <c r="D459" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -81023,13 +81159,13 @@
       <c r="DC459" s="13"/>
     </row>
     <row r="460" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A460" s="7">
+      <c r="A460" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B460" s="8"/>
-      <c r="C460" s="8"/>
-      <c r="D460" s="9">
+      <c r="B460" s="17"/>
+      <c r="C460" s="17"/>
+      <c r="D460" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -81257,13 +81393,13 @@
       <c r="DC460" s="13"/>
     </row>
     <row r="461" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A461" s="7">
+      <c r="A461" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B461" s="8"/>
-      <c r="C461" s="8"/>
-      <c r="D461" s="9">
+      <c r="B461" s="17"/>
+      <c r="C461" s="17"/>
+      <c r="D461" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -81479,13 +81615,13 @@
       <c r="DC461" s="13"/>
     </row>
     <row r="462" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A462" s="7">
+      <c r="A462" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B462" s="8"/>
-      <c r="C462" s="8"/>
-      <c r="D462" s="9">
+      <c r="B462" s="17"/>
+      <c r="C462" s="17"/>
+      <c r="D462" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -81720,13 +81856,13 @@
       <c r="DC462" s="13"/>
     </row>
     <row r="463" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A463" s="7">
+      <c r="A463" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B463" s="8"/>
-      <c r="C463" s="8"/>
-      <c r="D463" s="9">
+      <c r="B463" s="17"/>
+      <c r="C463" s="17"/>
+      <c r="D463" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -81947,13 +82083,13 @@
       <c r="DC463" s="13"/>
     </row>
     <row r="464" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A464" s="7">
+      <c r="A464" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B464" s="8"/>
-      <c r="C464" s="8"/>
-      <c r="D464" s="9">
+      <c r="B464" s="17"/>
+      <c r="C464" s="17"/>
+      <c r="D464" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -82187,13 +82323,13 @@
       <c r="DC464" s="13"/>
     </row>
     <row r="465" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A465" s="7">
+      <c r="A465" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B465" s="8"/>
-      <c r="C465" s="8"/>
-      <c r="D465" s="9">
+      <c r="B465" s="17"/>
+      <c r="C465" s="17"/>
+      <c r="D465" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -82406,13 +82542,13 @@
       <c r="DC465" s="13"/>
     </row>
     <row r="466" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A466" s="7">
+      <c r="A466" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B466" s="8"/>
-      <c r="C466" s="8"/>
-      <c r="D466" s="9">
+      <c r="B466" s="17"/>
+      <c r="C466" s="17"/>
+      <c r="D466" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -82629,13 +82765,13 @@
       <c r="DC466" s="13"/>
     </row>
     <row r="467" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A467" s="7">
+      <c r="A467" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B467" s="8"/>
-      <c r="C467" s="8"/>
-      <c r="D467" s="9">
+      <c r="B467" s="17"/>
+      <c r="C467" s="17"/>
+      <c r="D467" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -82854,13 +82990,13 @@
       <c r="DC467" s="13"/>
     </row>
     <row r="468" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A468" s="7">
+      <c r="A468" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B468" s="8"/>
-      <c r="C468" s="8"/>
-      <c r="D468" s="9">
+      <c r="B468" s="17"/>
+      <c r="C468" s="17"/>
+      <c r="D468" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -83084,13 +83220,13 @@
       <c r="DC468" s="13"/>
     </row>
     <row r="469" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A469" s="7">
+      <c r="A469" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B469" s="8"/>
-      <c r="C469" s="8"/>
-      <c r="D469" s="9">
+      <c r="B469" s="17"/>
+      <c r="C469" s="17"/>
+      <c r="D469" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -83318,13 +83454,13 @@
       <c r="DC469" s="13"/>
     </row>
     <row r="470" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A470" s="7">
+      <c r="A470" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B470" s="8"/>
-      <c r="C470" s="8"/>
-      <c r="D470" s="9">
+      <c r="B470" s="17"/>
+      <c r="C470" s="17"/>
+      <c r="D470" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -83545,13 +83681,13 @@
       <c r="DC470" s="13"/>
     </row>
     <row r="471" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A471" s="7">
+      <c r="A471" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B471" s="8"/>
-      <c r="C471" s="8"/>
-      <c r="D471" s="9">
+      <c r="B471" s="17"/>
+      <c r="C471" s="17"/>
+      <c r="D471" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -83797,13 +83933,13 @@
       <c r="DC471" s="13"/>
     </row>
     <row r="472" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A472" s="7">
+      <c r="A472" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B472" s="8"/>
-      <c r="C472" s="8"/>
-      <c r="D472" s="9">
+      <c r="B472" s="17"/>
+      <c r="C472" s="17"/>
+      <c r="D472" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -84023,13 +84159,13 @@
       <c r="DC472" s="13"/>
     </row>
     <row r="473" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A473" s="7">
+      <c r="A473" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B473" s="8"/>
-      <c r="C473" s="8"/>
-      <c r="D473" s="9">
+      <c r="B473" s="17"/>
+      <c r="C473" s="17"/>
+      <c r="D473" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -84246,13 +84382,13 @@
       <c r="DC473" s="13"/>
     </row>
     <row r="474" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A474" s="7">
+      <c r="A474" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B474" s="8"/>
-      <c r="C474" s="8"/>
-      <c r="D474" s="9">
+      <c r="B474" s="17"/>
+      <c r="C474" s="17"/>
+      <c r="D474" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -84473,13 +84609,13 @@
       <c r="DC474" s="13"/>
     </row>
     <row r="475" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A475" s="7">
+      <c r="A475" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B475" s="8"/>
-      <c r="C475" s="8"/>
-      <c r="D475" s="9">
+      <c r="B475" s="17"/>
+      <c r="C475" s="17"/>
+      <c r="D475" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -84705,13 +84841,13 @@
       <c r="DC475" s="13"/>
     </row>
     <row r="476" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A476" s="7">
+      <c r="A476" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B476" s="8"/>
-      <c r="C476" s="8"/>
-      <c r="D476" s="9">
+      <c r="B476" s="17"/>
+      <c r="C476" s="17"/>
+      <c r="D476" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -84943,13 +85079,13 @@
       <c r="DC476" s="13"/>
     </row>
     <row r="477" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A477" s="7">
+      <c r="A477" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B477" s="8"/>
-      <c r="C477" s="8"/>
-      <c r="D477" s="9">
+      <c r="B477" s="17"/>
+      <c r="C477" s="17"/>
+      <c r="D477" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -85162,13 +85298,13 @@
       <c r="DC477" s="13"/>
     </row>
     <row r="478" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A478" s="7">
+      <c r="A478" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B478" s="8"/>
-      <c r="C478" s="8"/>
-      <c r="D478" s="9">
+      <c r="B478" s="17"/>
+      <c r="C478" s="17"/>
+      <c r="D478" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -85396,13 +85532,13 @@
       <c r="DC478" s="13"/>
     </row>
     <row r="479" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A479" s="7">
+      <c r="A479" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B479" s="8"/>
-      <c r="C479" s="8"/>
-      <c r="D479" s="9">
+      <c r="B479" s="17"/>
+      <c r="C479" s="17"/>
+      <c r="D479" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -85641,13 +85777,13 @@
       <c r="DC479" s="13"/>
     </row>
     <row r="480" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A480" s="7">
+      <c r="A480" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B480" s="8"/>
-      <c r="C480" s="8"/>
-      <c r="D480" s="9">
+      <c r="B480" s="17"/>
+      <c r="C480" s="17"/>
+      <c r="D480" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -85882,15 +86018,15 @@
       <c r="DC480" s="13"/>
     </row>
     <row r="481" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A481" s="7">
+      <c r="A481" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B481" s="8" t="s">
+      <c r="B481" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="C481" s="8"/>
-      <c r="D481" s="9">
+      <c r="C481" s="17"/>
+      <c r="D481" s="18">
         <f t="shared" si="37"/>
         <v>30</v>
       </c>
@@ -86121,13 +86257,13 @@
       <c r="DC481" s="13"/>
     </row>
     <row r="482" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A482" s="7">
+      <c r="A482" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B482" s="8"/>
-      <c r="C482" s="8"/>
-      <c r="D482" s="9">
+      <c r="B482" s="17"/>
+      <c r="C482" s="17"/>
+      <c r="D482" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -86350,13 +86486,13 @@
       <c r="DC482" s="13"/>
     </row>
     <row r="483" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A483" s="7">
+      <c r="A483" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B483" s="8"/>
-      <c r="C483" s="8"/>
-      <c r="D483" s="9">
+      <c r="B483" s="17"/>
+      <c r="C483" s="17"/>
+      <c r="D483" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -86580,13 +86716,13 @@
       <c r="DC483" s="13"/>
     </row>
     <row r="484" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A484" s="7">
+      <c r="A484" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B484" s="8"/>
-      <c r="C484" s="8"/>
-      <c r="D484" s="9">
+      <c r="B484" s="17"/>
+      <c r="C484" s="17"/>
+      <c r="D484" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -86785,13 +86921,13 @@
       <c r="DC484" s="13"/>
     </row>
     <row r="485" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A485" s="7">
+      <c r="A485" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B485" s="8"/>
-      <c r="C485" s="8"/>
-      <c r="D485" s="9">
+      <c r="B485" s="17"/>
+      <c r="C485" s="17"/>
+      <c r="D485" s="18">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -87016,15 +87152,15 @@
       <c r="DC485" s="13"/>
     </row>
     <row r="486" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A486" s="7">
+      <c r="A486" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B486" s="8" t="s">
+      <c r="B486" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="C486" s="8"/>
-      <c r="D486" s="9">
+      <c r="C486" s="17"/>
+      <c r="D486" s="18">
         <f t="shared" si="37"/>
         <v>27</v>
       </c>
@@ -87247,15 +87383,15 @@
       <c r="DC486" s="13"/>
     </row>
     <row r="487" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A487" s="7">
+      <c r="A487" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B487" s="8" t="s">
+      <c r="B487" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="C487" s="8"/>
-      <c r="D487" s="9">
+      <c r="C487" s="17"/>
+      <c r="D487" s="18">
         <f t="shared" si="37"/>
         <v>24</v>
       </c>
@@ -87475,15 +87611,15 @@
       <c r="DC487" s="13"/>
     </row>
     <row r="488" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A488" s="7">
+      <c r="A488" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B488" s="8" t="s">
+      <c r="B488" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="C488" s="8"/>
-      <c r="D488" s="9">
+      <c r="C488" s="17"/>
+      <c r="D488" s="18">
         <f t="shared" si="37"/>
         <v>29</v>
       </c>
@@ -87726,15 +87862,15 @@
       <c r="DC488" s="13"/>
     </row>
     <row r="489" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A489" s="7">
+      <c r="A489" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B489" s="8" t="s">
+      <c r="B489" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="C489" s="8"/>
-      <c r="D489" s="9">
+      <c r="C489" s="17"/>
+      <c r="D489" s="18">
         <f t="shared" si="37"/>
         <v>28</v>
       </c>
@@ -87972,15 +88108,15 @@
       <c r="DC489" s="13"/>
     </row>
     <row r="490" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A490" s="7">
+      <c r="A490" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B490" s="8" t="s">
+      <c r="B490" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="C490" s="8"/>
-      <c r="D490" s="9">
+      <c r="C490" s="17"/>
+      <c r="D490" s="18">
         <f t="shared" si="37"/>
         <v>24</v>
       </c>
@@ -88192,15 +88328,15 @@
       <c r="DC490" s="13"/>
     </row>
     <row r="491" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A491" s="7">
+      <c r="A491" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B491" s="8" t="s">
+      <c r="B491" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="C491" s="8"/>
-      <c r="D491" s="9">
+      <c r="C491" s="17"/>
+      <c r="D491" s="18">
         <f t="shared" si="37"/>
         <v>24</v>
       </c>
@@ -88400,15 +88536,15 @@
       <c r="DC491" s="13"/>
     </row>
     <row r="492" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A492" s="7">
+      <c r="A492" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B492" s="8" t="s">
+      <c r="B492" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="C492" s="8"/>
-      <c r="D492" s="9">
+      <c r="C492" s="17"/>
+      <c r="D492" s="18">
         <f t="shared" si="37"/>
         <v>31</v>
       </c>
@@ -88641,15 +88777,15 @@
       <c r="DC492" s="13"/>
     </row>
     <row r="493" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A493" s="7">
+      <c r="A493" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B493" s="8" t="s">
+      <c r="B493" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="C493" s="8"/>
-      <c r="D493" s="9">
+      <c r="C493" s="17"/>
+      <c r="D493" s="18">
         <f t="shared" si="37"/>
         <v>37</v>
       </c>
@@ -88873,15 +89009,15 @@
       <c r="DC493" s="13"/>
     </row>
     <row r="494" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A494" s="7">
+      <c r="A494" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B494" s="8" t="s">
+      <c r="B494" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="C494" s="8"/>
-      <c r="D494" s="9">
+      <c r="C494" s="17"/>
+      <c r="D494" s="18">
         <f t="shared" si="37"/>
         <v>29</v>
       </c>
@@ -89132,15 +89268,15 @@
       <c r="DC494" s="13"/>
     </row>
     <row r="495" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A495" s="7">
+      <c r="A495" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B495" s="8" t="s">
+      <c r="B495" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="C495" s="8"/>
-      <c r="D495" s="9">
+      <c r="C495" s="17"/>
+      <c r="D495" s="18">
         <f t="shared" si="37"/>
         <v>28</v>
       </c>
@@ -89351,15 +89487,15 @@
       <c r="DC495" s="13"/>
     </row>
     <row r="496" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A496" s="7">
+      <c r="A496" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B496" s="8" t="s">
+      <c r="B496" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="C496" s="8"/>
-      <c r="D496" s="9">
+      <c r="C496" s="17"/>
+      <c r="D496" s="18">
         <f t="shared" si="37"/>
         <v>24</v>
       </c>
@@ -89590,15 +89726,15 @@
       <c r="DC496" s="13"/>
     </row>
     <row r="497" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A497" s="7">
+      <c r="A497" s="16">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B497" s="8" t="s">
+      <c r="B497" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="C497" s="8"/>
-      <c r="D497" s="9">
+      <c r="C497" s="17"/>
+      <c r="D497" s="18">
         <f t="shared" si="37"/>
         <v>20</v>
       </c>
@@ -89817,15 +89953,15 @@
       <c r="DC497" s="13"/>
     </row>
     <row r="498" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A498" s="7">
+      <c r="A498" s="16">
         <f t="shared" ref="A498" si="41">COUNTA(J498:O498)</f>
         <v>6</v>
       </c>
-      <c r="B498" s="8" t="s">
+      <c r="B498" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="C498" s="8"/>
-      <c r="D498" s="9">
+      <c r="C498" s="17"/>
+      <c r="D498" s="18">
         <f t="shared" ref="D498" si="42">LEN(B498)-LEN(SUBSTITUTE(B498,",",""))+1</f>
         <v>22</v>
       </c>
@@ -90051,15 +90187,15 @@
       <c r="DC498" s="13"/>
     </row>
     <row r="499" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A499" s="7">
+      <c r="A499" s="16">
         <f t="shared" ref="A499" si="45">COUNTA(J499:O499)</f>
         <v>6</v>
       </c>
-      <c r="B499" s="8" t="s">
+      <c r="B499" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="C499" s="8"/>
-      <c r="D499" s="9">
+      <c r="C499" s="17"/>
+      <c r="D499" s="18">
         <f t="shared" ref="D499" si="46">LEN(B499)-LEN(SUBSTITUTE(B499,",",""))+1</f>
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Levels16MoveList: update 400+ levels with 7x7 Level: fix a fatal bug that causes overlay to shift from s5d6 s6d6 and vice versa. Audio, AudioManager: Add boypain1...4, enemyflame. Particles and ParticleEngine: add DragonFireLite. Add ability to flip on xScale GameboardSprite: add RotateDirectionType enum for use in rotateOverlay() PlayerSprite: switch out dragon scratch animation with fire breath. Much cooler and makes more sense! GameEngine: move haptics with knockbackAnimation out of GameEngine and into said function in PlayerSprite.
</commit_message>
<xml_diff>
--- a/JSON/Levels16MoveList.xlsx
+++ b/JSON/Levels16MoveList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFEC3DC-2B04-9B4C-BD63-15406B8B3449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6686F1F5-4D44-4645-AA3F-73C8F6665D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36020" yWindow="-2400" windowWidth="51180" windowHeight="24180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19560" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19679" uniqueCount="298">
   <si>
     <t>health</t>
   </si>
@@ -913,6 +913,24 @@
   <si>
     <t>R,D,D,D,D,D,R,R,R,U,L,L,U,R,R,U,L,L,L,U,U,R,D,U,R,U,R,R</t>
   </si>
+  <si>
+    <t>R,D,R,D,R,D,L,U,U,L,U,D,D,D,D,L,U,R,U,U,U,D,R,R,R,R,U,L,D,L,L,L,U,D,R,D,R,R,D,L,D,R</t>
+  </si>
+  <si>
+    <t>D,D,U,R,D,L,U,R,L,D,R,U,L,D,L,D,D,R,R,L,U,U,U,R,U,R,R,D,D,U,L,L,U,R,R,U,D,D,L,L,R,R,D,R,U,L</t>
+  </si>
+  <si>
+    <t>D,D,R,U,L,R,D,R,R,R,D,R,L,U,L,L,U,D,U,D,U,L,R,D,D,D,R,D,R,R,R,D</t>
+  </si>
+  <si>
+    <t>R,D,D,D,U,U,U,L,R,U,D,D,D,U,U,U,D,L,R,U,U,R,D,D,D,D,D,D,R,R,R</t>
+  </si>
+  <si>
+    <t>R,R,L,U,R,D,L,D,U,L,D,R,L,D,U,L,D,R,U,D,R,D,L,U,U,R,D,D,U,U,U,R,R,R,R,R,R</t>
+  </si>
+  <si>
+    <t>YGBBGY</t>
+  </si>
 </sst>
 </file>
 
@@ -1473,7 +1491,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1509,12 +1527,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1875,10 +1887,10 @@
   <dimension ref="A1:DC499"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="BZ362" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="Z386" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B404" sqref="B404"/>
+      <selection pane="bottomRight" activeCell="C409" sqref="C409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1892,43 +1904,7 @@
     <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5" customWidth="1"/>
-    <col min="17" max="20" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.1640625" customWidth="1"/>
-    <col min="24" max="29" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.5" customWidth="1"/>
-    <col min="31" max="31" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.5" customWidth="1"/>
-    <col min="38" max="43" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.5" customWidth="1"/>
-    <col min="45" max="45" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.5" customWidth="1"/>
-    <col min="52" max="57" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="9.5" customWidth="1"/>
-    <col min="59" max="64" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.1640625" customWidth="1"/>
-    <col min="66" max="71" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.1640625" customWidth="1"/>
-    <col min="73" max="78" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="8.1640625" customWidth="1"/>
-    <col min="80" max="85" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="8.1640625" customWidth="1"/>
-    <col min="87" max="92" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="8.1640625" customWidth="1"/>
-    <col min="94" max="99" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="8.1640625" customWidth="1"/>
-    <col min="101" max="106" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="8.1640625" customWidth="1"/>
+    <col min="10" max="107" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:107" x14ac:dyDescent="0.2">
@@ -2256,7 +2232,7 @@
     </row>
     <row r="2" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
-        <f>COUNTA(J2:O2)</f>
+        <f>COUNTA(J2:P2)</f>
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2360,7 +2336,7 @@
     </row>
     <row r="3" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
-        <f t="shared" ref="A3:A66" si="0">COUNTA(J3:O3)</f>
+        <f t="shared" ref="A3:A66" si="0">COUNTA(J3:P3)</f>
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -9960,7 +9936,7 @@
     </row>
     <row r="67" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
-        <f t="shared" ref="A67:A130" si="6">COUNTA(J67:O67)</f>
+        <f t="shared" ref="A67:A130" si="6">COUNTA(J67:P67)</f>
         <v>3</v>
       </c>
       <c r="B67" s="8" t="s">
@@ -18296,7 +18272,7 @@
     </row>
     <row r="131" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
-        <f t="shared" ref="A131:A194" si="11">COUNTA(J131:O131)</f>
+        <f t="shared" ref="A131:A194" si="11">COUNTA(J131:P131)</f>
         <v>4</v>
       </c>
       <c r="B131" s="8" t="s">
@@ -27575,7 +27551,7 @@
     </row>
     <row r="195" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A195" s="7">
-        <f t="shared" ref="A195:A258" si="16">COUNTA(J195:O195)</f>
+        <f t="shared" ref="A195:A258" si="16">COUNTA(J195:P195)</f>
         <v>4</v>
       </c>
       <c r="B195" s="8"/>
@@ -38499,7 +38475,7 @@
     </row>
     <row r="259" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A259" s="7">
-        <f t="shared" ref="A259:A322" si="21">COUNTA(J259:O259)</f>
+        <f t="shared" ref="A259:A322" si="21">COUNTA(J259:P259)</f>
         <v>5</v>
       </c>
       <c r="B259" s="8" t="s">
@@ -51078,7 +51054,7 @@
     </row>
     <row r="323" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A323" s="7">
-        <f t="shared" ref="A323:A386" si="26">COUNTA(J323:O323)</f>
+        <f t="shared" ref="A323:A386" si="26">COUNTA(J323:P323)</f>
         <v>6</v>
       </c>
       <c r="B323" s="8"/>
@@ -64245,7 +64221,7 @@
     </row>
     <row r="387" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A387" s="7">
-        <f t="shared" ref="A387:A450" si="31">COUNTA(J387:O387)</f>
+        <f t="shared" ref="A387:A450" si="31">COUNTA(J387:P387)</f>
         <v>6</v>
       </c>
       <c r="B387" s="8"/>
@@ -67721,9 +67697,9 @@
       <c r="DC402" s="13"/>
     </row>
     <row r="403" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A403" s="7">
+      <c r="A403" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B403" s="8" t="s">
         <v>290</v>
@@ -67999,9 +67975,9 @@
       <c r="DC403" s="13"/>
     </row>
     <row r="404" spans="1:107" x14ac:dyDescent="0.2">
-      <c r="A404" s="7">
+      <c r="A404" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B404" s="8" t="s">
         <v>291</v>
@@ -68311,17 +68287,19 @@
     <row r="405" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A405" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B405" s="17"/>
-      <c r="C405" s="17"/>
-      <c r="D405" s="18">
+        <v>7</v>
+      </c>
+      <c r="B405" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C405" s="8"/>
+      <c r="D405" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="E405" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F405" s="10">
         <f t="shared" si="34"/>
@@ -68332,7 +68310,7 @@
         <v>403</v>
       </c>
       <c r="H405" s="11">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="I405" s="11">
         <v>1</v>
@@ -68355,6 +68333,9 @@
       <c r="O405" t="s">
         <v>76</v>
       </c>
+      <c r="P405" t="s">
+        <v>76</v>
+      </c>
       <c r="Q405" s="12" t="s">
         <v>76</v>
       </c>
@@ -68373,7 +68354,9 @@
       <c r="V405" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W405" s="12"/>
+      <c r="W405" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X405" t="s">
         <v>76</v>
       </c>
@@ -68392,6 +68375,9 @@
       <c r="AC405" t="s">
         <v>76</v>
       </c>
+      <c r="AD405" t="s">
+        <v>76</v>
+      </c>
       <c r="AE405" s="12" t="s">
         <v>76</v>
       </c>
@@ -68410,7 +68396,9 @@
       <c r="AJ405" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK405" s="12"/>
+      <c r="AK405" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL405" t="s">
         <v>76</v>
       </c>
@@ -68429,6 +68417,9 @@
       <c r="AQ405" t="s">
         <v>76</v>
       </c>
+      <c r="AR405" t="s">
+        <v>76</v>
+      </c>
       <c r="AS405" s="12" t="s">
         <v>76</v>
       </c>
@@ -68445,9 +68436,32 @@
         <v>76</v>
       </c>
       <c r="AX405" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY405" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ405" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA405" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB405" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC405" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD405" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE405" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF405" t="s">
         <v>77</v>
       </c>
-      <c r="AY405" s="12"/>
       <c r="BG405" s="13"/>
       <c r="BH405" s="13"/>
       <c r="BI405" s="13" t="s">
@@ -68460,7 +68474,9 @@
       <c r="BL405" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="BM405" s="13"/>
+      <c r="BM405" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="BO405" t="s">
         <v>82</v>
       </c>
@@ -68476,6 +68492,9 @@
       <c r="BS405" t="s">
         <v>78</v>
       </c>
+      <c r="BT405" t="s">
+        <v>78</v>
+      </c>
       <c r="BU405" s="13" t="s">
         <v>79</v>
       </c>
@@ -68494,7 +68513,9 @@
       <c r="BZ405" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="CA405" s="13"/>
+      <c r="CA405" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="CC405" t="s">
         <v>82</v>
       </c>
@@ -68510,6 +68531,9 @@
       <c r="CG405" t="s">
         <v>79</v>
       </c>
+      <c r="CH405" t="s">
+        <v>79</v>
+      </c>
       <c r="CI405" s="13" t="s">
         <v>79</v>
       </c>
@@ -68544,28 +68568,43 @@
       <c r="CT405" t="s">
         <v>80</v>
       </c>
-      <c r="CW405" s="13"/>
-      <c r="CX405" s="13"/>
-      <c r="CY405" s="13"/>
-      <c r="CZ405" s="13"/>
+      <c r="CV405" t="s">
+        <v>78</v>
+      </c>
+      <c r="CW405" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CX405" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CY405" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CZ405" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="DA405" s="13"/>
-      <c r="DB405" s="13"/>
+      <c r="DB405" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="DC405" s="13"/>
     </row>
     <row r="406" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A406" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B406" s="17"/>
-      <c r="C406" s="17"/>
-      <c r="D406" s="18">
+        <v>7</v>
+      </c>
+      <c r="B406" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C406" s="8"/>
+      <c r="D406" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="E406" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F406" s="10">
         <f t="shared" si="34"/>
@@ -68576,7 +68615,7 @@
         <v>404</v>
       </c>
       <c r="H406" s="11">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="I406" s="11">
         <v>1</v>
@@ -68599,6 +68638,9 @@
       <c r="O406" t="s">
         <v>76</v>
       </c>
+      <c r="P406" t="s">
+        <v>76</v>
+      </c>
       <c r="Q406" s="12" t="s">
         <v>76</v>
       </c>
@@ -68617,7 +68659,9 @@
       <c r="V406" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W406" s="12"/>
+      <c r="W406" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X406" t="s">
         <v>76</v>
       </c>
@@ -68636,6 +68680,9 @@
       <c r="AC406" t="s">
         <v>76</v>
       </c>
+      <c r="AD406" t="s">
+        <v>76</v>
+      </c>
       <c r="AE406" s="12" t="s">
         <v>76</v>
       </c>
@@ -68654,7 +68701,9 @@
       <c r="AJ406" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK406" s="12"/>
+      <c r="AK406" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL406" t="s">
         <v>76</v>
       </c>
@@ -68671,6 +68720,9 @@
         <v>76</v>
       </c>
       <c r="AQ406" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR406" t="s">
         <v>76</v>
       </c>
       <c r="AS406" s="12" t="s">
@@ -68691,7 +68743,30 @@
       <c r="AX406" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="AY406" s="12"/>
+      <c r="AY406" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ406" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA406" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB406" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC406" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD406" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE406" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF406" t="s">
+        <v>76</v>
+      </c>
       <c r="BG406" s="13"/>
       <c r="BH406" s="13"/>
       <c r="BI406" s="13" t="s">
@@ -68704,7 +68779,9 @@
         <v>78</v>
       </c>
       <c r="BL406" s="13"/>
-      <c r="BM406" s="13"/>
+      <c r="BM406" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="BO406" t="s">
         <v>87</v>
       </c>
@@ -68723,7 +68800,9 @@
       <c r="BU406" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BV406" s="13"/>
+      <c r="BV406" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="BW406" s="13" t="s">
         <v>79</v>
       </c>
@@ -68734,17 +68813,25 @@
       <c r="BZ406" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="CA406" s="13"/>
+      <c r="CA406" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="CB406" t="s">
         <v>79</v>
       </c>
       <c r="CC406" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CE406" t="s">
         <v>79</v>
       </c>
       <c r="CF406" t="s">
+        <v>79</v>
+      </c>
+      <c r="CG406" t="s">
+        <v>78</v>
+      </c>
+      <c r="CH406" t="s">
         <v>79</v>
       </c>
       <c r="CI406" s="13" t="s">
@@ -68762,41 +68849,53 @@
       <c r="CM406" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="CN406" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CO406" s="13"/>
+      <c r="CN406" s="13"/>
+      <c r="CO406" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="CQ406" t="s">
         <v>78</v>
       </c>
       <c r="CR406" t="s">
         <v>79</v>
       </c>
-      <c r="CT406" t="s">
-        <v>78</v>
-      </c>
-      <c r="CW406" s="13"/>
+      <c r="CS406" t="s">
+        <v>78</v>
+      </c>
+      <c r="CW406" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="CX406" s="13"/>
-      <c r="CY406" s="13"/>
-      <c r="CZ406" s="13"/>
-      <c r="DA406" s="13"/>
+      <c r="CY406" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CZ406" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="DA406" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="DB406" s="13"/>
-      <c r="DC406" s="13"/>
+      <c r="DC406" s="13" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="407" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A407" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B407" s="17"/>
-      <c r="C407" s="17"/>
-      <c r="D407" s="18">
+        <v>7</v>
+      </c>
+      <c r="B407" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C407" s="8"/>
+      <c r="D407" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E407" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F407" s="10">
         <f t="shared" si="34"/>
@@ -68807,7 +68906,7 @@
         <v>405</v>
       </c>
       <c r="H407" s="11">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I407" s="11">
         <v>1</v>
@@ -68830,6 +68929,9 @@
       <c r="O407" t="s">
         <v>76</v>
       </c>
+      <c r="P407" t="s">
+        <v>76</v>
+      </c>
       <c r="Q407" s="12" t="s">
         <v>76</v>
       </c>
@@ -68848,7 +68950,9 @@
       <c r="V407" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W407" s="12"/>
+      <c r="W407" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X407" t="s">
         <v>76</v>
       </c>
@@ -68867,6 +68971,9 @@
       <c r="AC407" t="s">
         <v>76</v>
       </c>
+      <c r="AD407" t="s">
+        <v>76</v>
+      </c>
       <c r="AE407" s="12" t="s">
         <v>76</v>
       </c>
@@ -68885,7 +68992,9 @@
       <c r="AJ407" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK407" s="12"/>
+      <c r="AK407" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL407" t="s">
         <v>76</v>
       </c>
@@ -68904,6 +69013,9 @@
       <c r="AQ407" t="s">
         <v>76</v>
       </c>
+      <c r="AR407" t="s">
+        <v>76</v>
+      </c>
       <c r="AS407" s="12" t="s">
         <v>76</v>
       </c>
@@ -68920,9 +69032,32 @@
         <v>76</v>
       </c>
       <c r="AX407" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY407" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ407" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA407" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB407" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC407" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD407" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE407" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF407" t="s">
         <v>77</v>
       </c>
-      <c r="AY407" s="12"/>
       <c r="BG407" s="13"/>
       <c r="BH407" s="13"/>
       <c r="BI407" s="13" t="s">
@@ -68951,6 +69086,9 @@
       <c r="BS407" t="s">
         <v>82</v>
       </c>
+      <c r="BT407" t="s">
+        <v>79</v>
+      </c>
       <c r="BU407" s="13"/>
       <c r="BV407" s="13" t="s">
         <v>87</v>
@@ -68967,7 +69105,9 @@
       <c r="BZ407" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="CA407" s="13"/>
+      <c r="CA407" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="CB407" t="s">
         <v>79</v>
       </c>
@@ -68986,9 +69126,10 @@
       <c r="CG407" t="s">
         <v>78</v>
       </c>
-      <c r="CI407" s="13" t="s">
-        <v>79</v>
-      </c>
+      <c r="CH407" t="s">
+        <v>79</v>
+      </c>
+      <c r="CI407" s="13"/>
       <c r="CJ407" s="13" t="s">
         <v>79</v>
       </c>
@@ -69018,12 +69159,20 @@
         <v>78</v>
       </c>
       <c r="CT407" t="s">
-        <v>78</v>
-      </c>
-      <c r="CW407" s="13"/>
-      <c r="CX407" s="13"/>
-      <c r="CY407" s="13"/>
-      <c r="CZ407" s="13"/>
+        <v>79</v>
+      </c>
+      <c r="CW407" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CX407" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CY407" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CZ407" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="DA407" s="13"/>
       <c r="DB407" s="13"/>
       <c r="DC407" s="13"/>
@@ -69031,17 +69180,19 @@
     <row r="408" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A408" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B408" s="17"/>
-      <c r="C408" s="17"/>
-      <c r="D408" s="18">
+        <v>7</v>
+      </c>
+      <c r="B408" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="C408" s="8"/>
+      <c r="D408" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E408" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F408" s="10">
         <f t="shared" si="34"/>
@@ -69052,7 +69203,7 @@
         <v>406</v>
       </c>
       <c r="H408" s="11">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I408" s="11">
         <v>1</v>
@@ -69075,6 +69226,9 @@
       <c r="O408" t="s">
         <v>76</v>
       </c>
+      <c r="P408" t="s">
+        <v>76</v>
+      </c>
       <c r="Q408" s="12" t="s">
         <v>76</v>
       </c>
@@ -69093,7 +69247,9 @@
       <c r="V408" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W408" s="12"/>
+      <c r="W408" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X408" t="s">
         <v>76</v>
       </c>
@@ -69112,6 +69268,9 @@
       <c r="AC408" t="s">
         <v>76</v>
       </c>
+      <c r="AD408" t="s">
+        <v>76</v>
+      </c>
       <c r="AE408" s="12" t="s">
         <v>76</v>
       </c>
@@ -69130,7 +69289,9 @@
       <c r="AJ408" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK408" s="12"/>
+      <c r="AK408" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL408" t="s">
         <v>76</v>
       </c>
@@ -69149,6 +69310,9 @@
       <c r="AQ408" t="s">
         <v>76</v>
       </c>
+      <c r="AR408" t="s">
+        <v>76</v>
+      </c>
       <c r="AS408" s="12" t="s">
         <v>76</v>
       </c>
@@ -69165,9 +69329,32 @@
         <v>76</v>
       </c>
       <c r="AX408" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY408" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ408" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA408" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB408" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC408" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD408" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE408" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF408" t="s">
         <v>77</v>
       </c>
-      <c r="AY408" s="12"/>
       <c r="BG408" s="13"/>
       <c r="BH408" s="13" t="s">
         <v>82</v>
@@ -69178,13 +69365,13 @@
       <c r="BJ408" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="BK408" s="13" t="s">
-        <v>79</v>
-      </c>
+      <c r="BK408" s="13"/>
       <c r="BL408" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM408" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="BM408" s="13"/>
       <c r="BN408" t="s">
         <v>79</v>
       </c>
@@ -69201,6 +69388,9 @@
         <v>79</v>
       </c>
       <c r="BS408" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT408" t="s">
         <v>82</v>
       </c>
       <c r="BU408" s="13" t="s">
@@ -69216,12 +69406,14 @@
         <v>86</v>
       </c>
       <c r="BY408" s="13" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="BZ408" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CA408" s="13"/>
+        <v>79</v>
+      </c>
+      <c r="CA408" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="CB408" t="s">
         <v>90</v>
       </c>
@@ -69235,9 +69427,12 @@
         <v>86</v>
       </c>
       <c r="CF408" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="CG408" t="s">
+        <v>79</v>
+      </c>
+      <c r="CH408" t="s">
         <v>78</v>
       </c>
       <c r="CI408" s="13" t="s">
@@ -69253,12 +69448,14 @@
         <v>86</v>
       </c>
       <c r="CM408" s="13" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="CN408" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="CO408" s="13"/>
+      <c r="CO408" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="CP408" t="s">
         <v>78</v>
       </c>
@@ -69269,33 +69466,53 @@
         <v>86</v>
       </c>
       <c r="CS408" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="CT408" t="s">
         <v>86</v>
       </c>
-      <c r="CW408" s="13"/>
-      <c r="CX408" s="13"/>
-      <c r="CY408" s="13"/>
-      <c r="CZ408" s="13"/>
-      <c r="DA408" s="13"/>
+      <c r="CU408" t="s">
+        <v>79</v>
+      </c>
+      <c r="CV408" t="s">
+        <v>79</v>
+      </c>
+      <c r="CW408" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CX408" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CY408" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="CZ408" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="DA408" s="13" t="s">
+        <v>86</v>
+      </c>
       <c r="DB408" s="13"/>
       <c r="DC408" s="13"/>
     </row>
     <row r="409" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A409" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B409" s="17"/>
-      <c r="C409" s="17"/>
-      <c r="D409" s="18">
+        <v>7</v>
+      </c>
+      <c r="B409" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="C409" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="D409" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="E409" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F409" s="10">
         <f t="shared" si="34"/>
@@ -69306,7 +69523,7 @@
         <v>407</v>
       </c>
       <c r="H409" s="11">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I409" s="11">
         <v>1</v>
@@ -69329,6 +69546,9 @@
       <c r="O409" t="s">
         <v>76</v>
       </c>
+      <c r="P409" t="s">
+        <v>76</v>
+      </c>
       <c r="Q409" s="12" t="s">
         <v>76</v>
       </c>
@@ -69347,7 +69567,9 @@
       <c r="V409" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W409" s="12"/>
+      <c r="W409" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X409" t="s">
         <v>76</v>
       </c>
@@ -69366,6 +69588,9 @@
       <c r="AC409" t="s">
         <v>76</v>
       </c>
+      <c r="AD409" t="s">
+        <v>76</v>
+      </c>
       <c r="AE409" s="12" t="s">
         <v>76</v>
       </c>
@@ -69384,7 +69609,9 @@
       <c r="AJ409" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK409" s="12"/>
+      <c r="AK409" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL409" t="s">
         <v>76</v>
       </c>
@@ -69403,6 +69630,9 @@
       <c r="AQ409" t="s">
         <v>76</v>
       </c>
+      <c r="AR409" t="s">
+        <v>76</v>
+      </c>
       <c r="AS409" s="12" t="s">
         <v>76</v>
       </c>
@@ -69419,9 +69649,32 @@
         <v>76</v>
       </c>
       <c r="AX409" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY409" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ409" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA409" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB409" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC409" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD409" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE409" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF409" t="s">
         <v>77</v>
       </c>
-      <c r="AY409" s="12"/>
       <c r="BG409" s="13"/>
       <c r="BH409" s="13"/>
       <c r="BI409" s="13" t="s">
@@ -69430,11 +69683,13 @@
       <c r="BJ409" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="BK409" s="13"/>
-      <c r="BL409" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="BM409" s="13"/>
+      <c r="BK409" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL409" s="13"/>
+      <c r="BM409" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="BO409" t="s">
         <v>87</v>
       </c>
@@ -69444,10 +69699,10 @@
       <c r="BQ409" t="s">
         <v>79</v>
       </c>
-      <c r="BR409" t="s">
-        <v>78</v>
-      </c>
       <c r="BS409" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT409" t="s">
         <v>87</v>
       </c>
       <c r="BU409" s="13" t="s">
@@ -69466,9 +69721,11 @@
         <v>79</v>
       </c>
       <c r="BZ409" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CA409" s="13"/>
+        <v>79</v>
+      </c>
+      <c r="CA409" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="CB409" t="s">
         <v>79</v>
       </c>
@@ -69487,38 +69744,59 @@
       <c r="CG409" t="s">
         <v>79</v>
       </c>
-      <c r="CI409" s="13"/>
-      <c r="CJ409" s="13" t="s">
-        <v>78</v>
-      </c>
+      <c r="CH409" t="s">
+        <v>78</v>
+      </c>
+      <c r="CI409" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CJ409" s="13"/>
       <c r="CK409" s="13" t="s">
         <v>79</v>
       </c>
       <c r="CL409" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="CM409" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CN409" s="13"/>
-      <c r="CO409" s="13"/>
-      <c r="CP409" t="s">
-        <v>78</v>
+      <c r="CM409" s="13"/>
+      <c r="CN409" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CO409" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="CQ409" t="s">
+        <v>78</v>
+      </c>
+      <c r="CR409" t="s">
+        <v>79</v>
+      </c>
+      <c r="CS409" t="s">
+        <v>79</v>
+      </c>
+      <c r="CT409" t="s">
+        <v>79</v>
+      </c>
+      <c r="CU409" t="s">
+        <v>79</v>
+      </c>
+      <c r="CV409" t="s">
+        <v>79</v>
+      </c>
+      <c r="CW409" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CX409" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="CR409" t="s">
-        <v>78</v>
-      </c>
-      <c r="CS409" t="s">
-        <v>79</v>
-      </c>
-      <c r="CW409" s="13"/>
-      <c r="CX409" s="13"/>
-      <c r="CY409" s="13"/>
-      <c r="CZ409" s="13"/>
-      <c r="DA409" s="13"/>
+      <c r="CY409" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CZ409" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="DA409" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="DB409" s="13"/>
       <c r="DC409" s="13"/>
     </row>
@@ -69527,9 +69805,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B410" s="17"/>
-      <c r="C410" s="17"/>
-      <c r="D410" s="18">
+      <c r="B410" s="8"/>
+      <c r="C410" s="8"/>
+      <c r="D410" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -69771,9 +70049,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B411" s="17"/>
-      <c r="C411" s="17"/>
-      <c r="D411" s="18">
+      <c r="B411" s="8"/>
+      <c r="C411" s="8"/>
+      <c r="D411" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -70000,9 +70278,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B412" s="17"/>
-      <c r="C412" s="17"/>
-      <c r="D412" s="18">
+      <c r="B412" s="8"/>
+      <c r="C412" s="8"/>
+      <c r="D412" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -70254,9 +70532,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B413" s="17"/>
-      <c r="C413" s="17"/>
-      <c r="D413" s="18">
+      <c r="B413" s="8"/>
+      <c r="C413" s="8"/>
+      <c r="D413" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -70508,9 +70786,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B414" s="17"/>
-      <c r="C414" s="17"/>
-      <c r="D414" s="18">
+      <c r="B414" s="8"/>
+      <c r="C414" s="8"/>
+      <c r="D414" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -70748,9 +71026,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B415" s="17"/>
-      <c r="C415" s="17"/>
-      <c r="D415" s="18">
+      <c r="B415" s="8"/>
+      <c r="C415" s="8"/>
+      <c r="D415" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -70994,9 +71272,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B416" s="17"/>
-      <c r="C416" s="17"/>
-      <c r="D416" s="18">
+      <c r="B416" s="8"/>
+      <c r="C416" s="8"/>
+      <c r="D416" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -71225,9 +71503,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B417" s="17"/>
-      <c r="C417" s="17"/>
-      <c r="D417" s="18">
+      <c r="B417" s="8"/>
+      <c r="C417" s="8"/>
+      <c r="D417" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -71471,9 +71749,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B418" s="17"/>
-      <c r="C418" s="17"/>
-      <c r="D418" s="18">
+      <c r="B418" s="8"/>
+      <c r="C418" s="8"/>
+      <c r="D418" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -71725,9 +72003,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B419" s="17"/>
-      <c r="C419" s="17"/>
-      <c r="D419" s="18">
+      <c r="B419" s="8"/>
+      <c r="C419" s="8"/>
+      <c r="D419" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -71964,9 +72242,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B420" s="17"/>
-      <c r="C420" s="17"/>
-      <c r="D420" s="18">
+      <c r="B420" s="8"/>
+      <c r="C420" s="8"/>
+      <c r="D420" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -72213,9 +72491,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B421" s="17"/>
-      <c r="C421" s="17"/>
-      <c r="D421" s="18">
+      <c r="B421" s="8"/>
+      <c r="C421" s="8"/>
+      <c r="D421" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -72427,9 +72705,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B422" s="17"/>
-      <c r="C422" s="17"/>
-      <c r="D422" s="18">
+      <c r="B422" s="8"/>
+      <c r="C422" s="8"/>
+      <c r="D422" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -72667,9 +72945,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B423" s="17"/>
-      <c r="C423" s="17"/>
-      <c r="D423" s="18">
+      <c r="B423" s="8"/>
+      <c r="C423" s="8"/>
+      <c r="D423" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -72904,9 +73182,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B424" s="17"/>
-      <c r="C424" s="17"/>
-      <c r="D424" s="18">
+      <c r="B424" s="8"/>
+      <c r="C424" s="8"/>
+      <c r="D424" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -73119,9 +73397,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B425" s="17"/>
-      <c r="C425" s="17"/>
-      <c r="D425" s="18">
+      <c r="B425" s="8"/>
+      <c r="C425" s="8"/>
+      <c r="D425" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -73373,9 +73651,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B426" s="17"/>
-      <c r="C426" s="17"/>
-      <c r="D426" s="18">
+      <c r="B426" s="8"/>
+      <c r="C426" s="8"/>
+      <c r="D426" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -73625,9 +73903,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B427" s="17"/>
-      <c r="C427" s="17"/>
-      <c r="D427" s="18">
+      <c r="B427" s="8"/>
+      <c r="C427" s="8"/>
+      <c r="D427" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -73852,9 +74130,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B428" s="17"/>
-      <c r="C428" s="17"/>
-      <c r="D428" s="18">
+      <c r="B428" s="8"/>
+      <c r="C428" s="8"/>
+      <c r="D428" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -74059,9 +74337,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B429" s="17"/>
-      <c r="C429" s="17"/>
-      <c r="D429" s="18">
+      <c r="B429" s="8"/>
+      <c r="C429" s="8"/>
+      <c r="D429" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -74285,9 +74563,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B430" s="17"/>
-      <c r="C430" s="17"/>
-      <c r="D430" s="18">
+      <c r="B430" s="8"/>
+      <c r="C430" s="8"/>
+      <c r="D430" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -74529,9 +74807,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B431" s="17"/>
-      <c r="C431" s="17"/>
-      <c r="D431" s="18">
+      <c r="B431" s="8"/>
+      <c r="C431" s="8"/>
+      <c r="D431" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -74759,9 +75037,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B432" s="17"/>
-      <c r="C432" s="17"/>
-      <c r="D432" s="18">
+      <c r="B432" s="8"/>
+      <c r="C432" s="8"/>
+      <c r="D432" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -75007,9 +75285,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B433" s="17"/>
-      <c r="C433" s="17"/>
-      <c r="D433" s="18">
+      <c r="B433" s="8"/>
+      <c r="C433" s="8"/>
+      <c r="D433" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -75255,9 +75533,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B434" s="17"/>
-      <c r="C434" s="17"/>
-      <c r="D434" s="18">
+      <c r="B434" s="8"/>
+      <c r="C434" s="8"/>
+      <c r="D434" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -75491,9 +75769,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B435" s="17"/>
-      <c r="C435" s="17"/>
-      <c r="D435" s="18">
+      <c r="B435" s="8"/>
+      <c r="C435" s="8"/>
+      <c r="D435" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -75721,9 +75999,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B436" s="17"/>
-      <c r="C436" s="17"/>
-      <c r="D436" s="18">
+      <c r="B436" s="8"/>
+      <c r="C436" s="8"/>
+      <c r="D436" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -75961,9 +76239,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B437" s="17"/>
-      <c r="C437" s="17"/>
-      <c r="D437" s="18">
+      <c r="B437" s="8"/>
+      <c r="C437" s="8"/>
+      <c r="D437" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -76206,9 +76484,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B438" s="17"/>
-      <c r="C438" s="17"/>
-      <c r="D438" s="18">
+      <c r="B438" s="8"/>
+      <c r="C438" s="8"/>
+      <c r="D438" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -76427,9 +76705,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B439" s="17"/>
-      <c r="C439" s="17"/>
-      <c r="D439" s="18">
+      <c r="B439" s="8"/>
+      <c r="C439" s="8"/>
+      <c r="D439" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -76650,9 +76928,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B440" s="17"/>
-      <c r="C440" s="17"/>
-      <c r="D440" s="18">
+      <c r="B440" s="8"/>
+      <c r="C440" s="8"/>
+      <c r="D440" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -76891,9 +77169,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B441" s="17"/>
-      <c r="C441" s="17"/>
-      <c r="D441" s="18">
+      <c r="B441" s="8"/>
+      <c r="C441" s="8"/>
+      <c r="D441" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -77120,9 +77398,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B442" s="17"/>
-      <c r="C442" s="17"/>
-      <c r="D442" s="18">
+      <c r="B442" s="8"/>
+      <c r="C442" s="8"/>
+      <c r="D442" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -77374,9 +77652,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B443" s="17"/>
-      <c r="C443" s="17"/>
-      <c r="D443" s="18">
+      <c r="B443" s="8"/>
+      <c r="C443" s="8"/>
+      <c r="D443" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -77589,9 +77867,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B444" s="17"/>
-      <c r="C444" s="17"/>
-      <c r="D444" s="18">
+      <c r="B444" s="8"/>
+      <c r="C444" s="8"/>
+      <c r="D444" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -77813,9 +78091,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B445" s="17"/>
-      <c r="C445" s="17"/>
-      <c r="D445" s="18">
+      <c r="B445" s="8"/>
+      <c r="C445" s="8"/>
+      <c r="D445" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -78063,9 +78341,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B446" s="17"/>
-      <c r="C446" s="17"/>
-      <c r="D446" s="18">
+      <c r="B446" s="8"/>
+      <c r="C446" s="8"/>
+      <c r="D446" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -78301,9 +78579,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B447" s="17"/>
-      <c r="C447" s="17"/>
-      <c r="D447" s="18">
+      <c r="B447" s="8"/>
+      <c r="C447" s="8"/>
+      <c r="D447" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -78525,9 +78803,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B448" s="17"/>
-      <c r="C448" s="17"/>
-      <c r="D448" s="18">
+      <c r="B448" s="8"/>
+      <c r="C448" s="8"/>
+      <c r="D448" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -78731,9 +79009,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B449" s="17"/>
-      <c r="C449" s="17"/>
-      <c r="D449" s="18">
+      <c r="B449" s="8"/>
+      <c r="C449" s="8"/>
+      <c r="D449" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -78970,9 +79248,9 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B450" s="17"/>
-      <c r="C450" s="17"/>
-      <c r="D450" s="18">
+      <c r="B450" s="8"/>
+      <c r="C450" s="8"/>
+      <c r="D450" s="9">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -79189,12 +79467,12 @@
     </row>
     <row r="451" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A451" s="16">
-        <f t="shared" ref="A451:A497" si="36">COUNTA(J451:O451)</f>
+        <f t="shared" ref="A451:A499" si="36">COUNTA(J451:P451)</f>
         <v>6</v>
       </c>
-      <c r="B451" s="17"/>
-      <c r="C451" s="17"/>
-      <c r="D451" s="18">
+      <c r="B451" s="8"/>
+      <c r="C451" s="8"/>
+      <c r="D451" s="9">
         <f t="shared" ref="D451:D497" si="37">LEN(B451)-LEN(SUBSTITUTE(B451,",",""))+1</f>
         <v>1</v>
       </c>
@@ -79401,9 +79679,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B452" s="17"/>
-      <c r="C452" s="17"/>
-      <c r="D452" s="18">
+      <c r="B452" s="8"/>
+      <c r="C452" s="8"/>
+      <c r="D452" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -79615,9 +79893,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B453" s="17"/>
-      <c r="C453" s="17"/>
-      <c r="D453" s="18">
+      <c r="B453" s="8"/>
+      <c r="C453" s="8"/>
+      <c r="D453" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -79835,9 +80113,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B454" s="17"/>
-      <c r="C454" s="17"/>
-      <c r="D454" s="18">
+      <c r="B454" s="8"/>
+      <c r="C454" s="8"/>
+      <c r="D454" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -80064,9 +80342,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B455" s="17"/>
-      <c r="C455" s="17"/>
-      <c r="D455" s="18">
+      <c r="B455" s="8"/>
+      <c r="C455" s="8"/>
+      <c r="D455" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -80291,9 +80569,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B456" s="17"/>
-      <c r="C456" s="17"/>
-      <c r="D456" s="18">
+      <c r="B456" s="8"/>
+      <c r="C456" s="8"/>
+      <c r="D456" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -80515,9 +80793,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B457" s="17"/>
-      <c r="C457" s="17"/>
-      <c r="D457" s="18">
+      <c r="B457" s="8"/>
+      <c r="C457" s="8"/>
+      <c r="D457" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -80742,9 +81020,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B458" s="17"/>
-      <c r="C458" s="17"/>
-      <c r="D458" s="18">
+      <c r="B458" s="8"/>
+      <c r="C458" s="8"/>
+      <c r="D458" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -80948,9 +81226,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B459" s="17"/>
-      <c r="C459" s="17"/>
-      <c r="D459" s="18">
+      <c r="B459" s="8"/>
+      <c r="C459" s="8"/>
+      <c r="D459" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -81163,9 +81441,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B460" s="17"/>
-      <c r="C460" s="17"/>
-      <c r="D460" s="18">
+      <c r="B460" s="8"/>
+      <c r="C460" s="8"/>
+      <c r="D460" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -81397,9 +81675,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B461" s="17"/>
-      <c r="C461" s="17"/>
-      <c r="D461" s="18">
+      <c r="B461" s="8"/>
+      <c r="C461" s="8"/>
+      <c r="D461" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -81619,9 +81897,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B462" s="17"/>
-      <c r="C462" s="17"/>
-      <c r="D462" s="18">
+      <c r="B462" s="8"/>
+      <c r="C462" s="8"/>
+      <c r="D462" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -81860,9 +82138,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B463" s="17"/>
-      <c r="C463" s="17"/>
-      <c r="D463" s="18">
+      <c r="B463" s="8"/>
+      <c r="C463" s="8"/>
+      <c r="D463" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -82087,9 +82365,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B464" s="17"/>
-      <c r="C464" s="17"/>
-      <c r="D464" s="18">
+      <c r="B464" s="8"/>
+      <c r="C464" s="8"/>
+      <c r="D464" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -82327,9 +82605,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B465" s="17"/>
-      <c r="C465" s="17"/>
-      <c r="D465" s="18">
+      <c r="B465" s="8"/>
+      <c r="C465" s="8"/>
+      <c r="D465" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -82546,9 +82824,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B466" s="17"/>
-      <c r="C466" s="17"/>
-      <c r="D466" s="18">
+      <c r="B466" s="8"/>
+      <c r="C466" s="8"/>
+      <c r="D466" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -82769,9 +83047,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B467" s="17"/>
-      <c r="C467" s="17"/>
-      <c r="D467" s="18">
+      <c r="B467" s="8"/>
+      <c r="C467" s="8"/>
+      <c r="D467" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -82994,9 +83272,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B468" s="17"/>
-      <c r="C468" s="17"/>
-      <c r="D468" s="18">
+      <c r="B468" s="8"/>
+      <c r="C468" s="8"/>
+      <c r="D468" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -83224,9 +83502,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B469" s="17"/>
-      <c r="C469" s="17"/>
-      <c r="D469" s="18">
+      <c r="B469" s="8"/>
+      <c r="C469" s="8"/>
+      <c r="D469" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -83458,9 +83736,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B470" s="17"/>
-      <c r="C470" s="17"/>
-      <c r="D470" s="18">
+      <c r="B470" s="8"/>
+      <c r="C470" s="8"/>
+      <c r="D470" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -83685,9 +83963,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B471" s="17"/>
-      <c r="C471" s="17"/>
-      <c r="D471" s="18">
+      <c r="B471" s="8"/>
+      <c r="C471" s="8"/>
+      <c r="D471" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -83937,9 +84215,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B472" s="17"/>
-      <c r="C472" s="17"/>
-      <c r="D472" s="18">
+      <c r="B472" s="8"/>
+      <c r="C472" s="8"/>
+      <c r="D472" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -84163,9 +84441,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B473" s="17"/>
-      <c r="C473" s="17"/>
-      <c r="D473" s="18">
+      <c r="B473" s="8"/>
+      <c r="C473" s="8"/>
+      <c r="D473" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -84386,9 +84664,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B474" s="17"/>
-      <c r="C474" s="17"/>
-      <c r="D474" s="18">
+      <c r="B474" s="8"/>
+      <c r="C474" s="8"/>
+      <c r="D474" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -84613,9 +84891,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B475" s="17"/>
-      <c r="C475" s="17"/>
-      <c r="D475" s="18">
+      <c r="B475" s="8"/>
+      <c r="C475" s="8"/>
+      <c r="D475" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -84845,9 +85123,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B476" s="17"/>
-      <c r="C476" s="17"/>
-      <c r="D476" s="18">
+      <c r="B476" s="8"/>
+      <c r="C476" s="8"/>
+      <c r="D476" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -85083,9 +85361,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B477" s="17"/>
-      <c r="C477" s="17"/>
-      <c r="D477" s="18">
+      <c r="B477" s="8"/>
+      <c r="C477" s="8"/>
+      <c r="D477" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -85302,9 +85580,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B478" s="17"/>
-      <c r="C478" s="17"/>
-      <c r="D478" s="18">
+      <c r="B478" s="8"/>
+      <c r="C478" s="8"/>
+      <c r="D478" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -85536,9 +85814,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B479" s="17"/>
-      <c r="C479" s="17"/>
-      <c r="D479" s="18">
+      <c r="B479" s="8"/>
+      <c r="C479" s="8"/>
+      <c r="D479" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -85781,9 +86059,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B480" s="17"/>
-      <c r="C480" s="17"/>
-      <c r="D480" s="18">
+      <c r="B480" s="8"/>
+      <c r="C480" s="8"/>
+      <c r="D480" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -86022,11 +86300,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B481" s="17" t="s">
+      <c r="B481" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C481" s="17"/>
-      <c r="D481" s="18">
+      <c r="C481" s="8"/>
+      <c r="D481" s="9">
         <f t="shared" si="37"/>
         <v>30</v>
       </c>
@@ -86261,9 +86539,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B482" s="17"/>
-      <c r="C482" s="17"/>
-      <c r="D482" s="18">
+      <c r="B482" s="8"/>
+      <c r="C482" s="8"/>
+      <c r="D482" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -86490,9 +86768,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B483" s="17"/>
-      <c r="C483" s="17"/>
-      <c r="D483" s="18">
+      <c r="B483" s="8"/>
+      <c r="C483" s="8"/>
+      <c r="D483" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -86720,9 +86998,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B484" s="17"/>
-      <c r="C484" s="17"/>
-      <c r="D484" s="18">
+      <c r="B484" s="8"/>
+      <c r="C484" s="8"/>
+      <c r="D484" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -86925,9 +87203,9 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B485" s="17"/>
-      <c r="C485" s="17"/>
-      <c r="D485" s="18">
+      <c r="B485" s="8"/>
+      <c r="C485" s="8"/>
+      <c r="D485" s="9">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
@@ -87156,11 +87434,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B486" s="17" t="s">
+      <c r="B486" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="C486" s="17"/>
-      <c r="D486" s="18">
+      <c r="C486" s="8"/>
+      <c r="D486" s="9">
         <f t="shared" si="37"/>
         <v>27</v>
       </c>
@@ -87387,11 +87665,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B487" s="17" t="s">
+      <c r="B487" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="C487" s="17"/>
-      <c r="D487" s="18">
+      <c r="C487" s="8"/>
+      <c r="D487" s="9">
         <f t="shared" si="37"/>
         <v>24</v>
       </c>
@@ -87615,11 +87893,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B488" s="17" t="s">
+      <c r="B488" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="C488" s="17"/>
-      <c r="D488" s="18">
+      <c r="C488" s="8"/>
+      <c r="D488" s="9">
         <f t="shared" si="37"/>
         <v>29</v>
       </c>
@@ -87866,11 +88144,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B489" s="17" t="s">
+      <c r="B489" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="C489" s="17"/>
-      <c r="D489" s="18">
+      <c r="C489" s="8"/>
+      <c r="D489" s="9">
         <f t="shared" si="37"/>
         <v>28</v>
       </c>
@@ -88112,11 +88390,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B490" s="17" t="s">
+      <c r="B490" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="C490" s="17"/>
-      <c r="D490" s="18">
+      <c r="C490" s="8"/>
+      <c r="D490" s="9">
         <f t="shared" si="37"/>
         <v>24</v>
       </c>
@@ -88332,11 +88610,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B491" s="17" t="s">
+      <c r="B491" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="C491" s="17"/>
-      <c r="D491" s="18">
+      <c r="C491" s="8"/>
+      <c r="D491" s="9">
         <f t="shared" si="37"/>
         <v>24</v>
       </c>
@@ -88540,11 +88818,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B492" s="17" t="s">
+      <c r="B492" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="C492" s="17"/>
-      <c r="D492" s="18">
+      <c r="C492" s="8"/>
+      <c r="D492" s="9">
         <f t="shared" si="37"/>
         <v>31</v>
       </c>
@@ -88781,11 +89059,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B493" s="17" t="s">
+      <c r="B493" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="C493" s="17"/>
-      <c r="D493" s="18">
+      <c r="C493" s="8"/>
+      <c r="D493" s="9">
         <f t="shared" si="37"/>
         <v>37</v>
       </c>
@@ -89013,11 +89291,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B494" s="17" t="s">
+      <c r="B494" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="C494" s="17"/>
-      <c r="D494" s="18">
+      <c r="C494" s="8"/>
+      <c r="D494" s="9">
         <f t="shared" si="37"/>
         <v>29</v>
       </c>
@@ -89272,11 +89550,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B495" s="17" t="s">
+      <c r="B495" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="C495" s="17"/>
-      <c r="D495" s="18">
+      <c r="C495" s="8"/>
+      <c r="D495" s="9">
         <f t="shared" si="37"/>
         <v>28</v>
       </c>
@@ -89491,11 +89769,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B496" s="17" t="s">
+      <c r="B496" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="C496" s="17"/>
-      <c r="D496" s="18">
+      <c r="C496" s="8"/>
+      <c r="D496" s="9">
         <f t="shared" si="37"/>
         <v>24</v>
       </c>
@@ -89730,11 +90008,11 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B497" s="17" t="s">
+      <c r="B497" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="C497" s="17"/>
-      <c r="D497" s="18">
+      <c r="C497" s="8"/>
+      <c r="D497" s="9">
         <f t="shared" si="37"/>
         <v>20</v>
       </c>
@@ -89954,19 +90232,19 @@
     </row>
     <row r="498" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A498" s="16">
-        <f t="shared" ref="A498" si="41">COUNTA(J498:O498)</f>
+        <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B498" s="17" t="s">
+      <c r="B498" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="C498" s="17"/>
-      <c r="D498" s="18">
-        <f t="shared" ref="D498" si="42">LEN(B498)-LEN(SUBSTITUTE(B498,",",""))+1</f>
+      <c r="C498" s="8"/>
+      <c r="D498" s="9">
+        <f t="shared" ref="D498" si="41">LEN(B498)-LEN(SUBSTITUTE(B498,",",""))+1</f>
         <v>22</v>
       </c>
       <c r="E498" s="14" t="b">
-        <f t="shared" ref="E498" si="43">D498=H498</f>
+        <f t="shared" ref="E498" si="42">D498=H498</f>
         <v>0</v>
       </c>
       <c r="F498" s="10">
@@ -89974,7 +90252,7 @@
         <v>496</v>
       </c>
       <c r="G498" s="10">
-        <f t="shared" ref="G498" si="44">F498</f>
+        <f t="shared" ref="G498" si="43">F498</f>
         <v>496</v>
       </c>
       <c r="H498" s="11">
@@ -90188,19 +90466,19 @@
     </row>
     <row r="499" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A499" s="16">
-        <f t="shared" ref="A499" si="45">COUNTA(J499:O499)</f>
+        <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B499" s="17" t="s">
+      <c r="B499" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="C499" s="17"/>
-      <c r="D499" s="18">
-        <f t="shared" ref="D499" si="46">LEN(B499)-LEN(SUBSTITUTE(B499,",",""))+1</f>
+      <c r="C499" s="8"/>
+      <c r="D499" s="9">
+        <f t="shared" ref="D499" si="44">LEN(B499)-LEN(SUBSTITUTE(B499,",",""))+1</f>
         <v>27</v>
       </c>
       <c r="E499" s="14" t="b">
-        <f t="shared" ref="E499" si="47">D499=H499</f>
+        <f t="shared" ref="E499" si="45">D499=H499</f>
         <v>0</v>
       </c>
       <c r="F499" s="10">
@@ -90208,7 +90486,7 @@
         <v>497</v>
       </c>
       <c r="G499" s="10">
-        <f t="shared" ref="G499" si="48">F499</f>
+        <f t="shared" ref="G499" si="46">F499</f>
         <v>497</v>
       </c>
       <c r="H499" s="11">

</xml_diff>

<commit_message>
Update Levels16MoveList. Haptics: add haptic for warps GameEngine: add bloodOverlay that progressively gets more alpha -> 0.5 as you progress through the levels. Add haptics for .gem, .hammer, .sword, .heart, .warps
</commit_message>
<xml_diff>
--- a/JSON/Levels16MoveList.xlsx
+++ b/JSON/Levels16MoveList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6686F1F5-4D44-4645-AA3F-73C8F6665D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065EA185-4CD7-174E-B56D-E99F206E58D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36020" yWindow="-2400" windowWidth="51180" windowHeight="24180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csvjson" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19679" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19877" uniqueCount="309">
   <si>
     <t>health</t>
   </si>
@@ -931,6 +931,39 @@
   <si>
     <t>YGBBGY</t>
   </si>
+  <si>
+    <t>D,R,D,U,D,U,D,D,U,U,R,L,R,L,R,R,L,L,R,U,U,U,R,D,L,R,L,L,D,R,R</t>
+  </si>
+  <si>
+    <t>R,L,L,L,U,U,U,L,U,D,R,R,U,D,R,L,L,L,D,D,D,L,D,D,D,R,D,R,L,D,L,R,D</t>
+  </si>
+  <si>
+    <t>R,L,D,R,R,D,R,D,L,D,R,U,L,U,L,R,R,D,U,R,D,D,R,D,D,U,R,D</t>
+  </si>
+  <si>
+    <t>R,L,D,D,D,D,D,L,U,D,D,U,R,L,L,R,L,D,U,R,R,U,U,U,R,R,U,D,R,D,L,R,R,D,L,R,R,D,L,R,R,D,L,R</t>
+  </si>
+  <si>
+    <t>D,D,D,R,R,L,D,R,U,U,R,U,D,U,U,D,D,R,L,D,R,D,L,R,D,R</t>
+  </si>
+  <si>
+    <t>U,R,U,R,U,D,R,R,U,L,L,R,D,R,U,U,L,R,R,U,R,U</t>
+  </si>
+  <si>
+    <t>R,U,R,D,L,R,R,L,R,L,R,L,L,L,L,L,L,L,U,R,D,R,R,R,R,R,R,L,R,R,R</t>
+  </si>
+  <si>
+    <t>R,D,R,R,R,L,L,L,L,D,U,R,R,L,L,L,R,R,R,R,U,D,D,L,R</t>
+  </si>
+  <si>
+    <t>R,R,R,R,R,D,D,D,D,L,U,L,U,L,U,L,L,D,D,D,D,R,R,R,R,R</t>
+  </si>
+  <si>
+    <t>R,R,R,L,D,L,D,L,D,D,D,U,R,R,D,U,R,L,U,R,U,R,D,U,U,R,U,D,D,D,D,D,L,R</t>
+  </si>
+  <si>
+    <t>R,L,D,R,U,U,R,D,L,L,D,R,L,L,L,D,L,U,D,D,L,U,R,D</t>
+  </si>
 </sst>
 </file>
 
@@ -1491,7 +1524,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1529,6 +1562,13 @@
     <xf numFmtId="0" fontId="14" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1886,11 +1926,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DC499"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="Z386" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="10" ySplit="2" topLeftCell="K401" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C409" sqref="C409"/>
+      <selection pane="bottomRight" activeCell="E419" sqref="E419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46425,15 +46465,17 @@
         <f t="shared" si="21"/>
         <v>6</v>
       </c>
-      <c r="B303" s="8"/>
+      <c r="B303" s="18" t="s">
+        <v>306</v>
+      </c>
       <c r="C303" s="8"/>
       <c r="D303" s="9">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E303" s="9" t="b">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F303" s="10">
         <f t="shared" si="24"/>
@@ -46679,15 +46721,17 @@
         <f t="shared" si="21"/>
         <v>6</v>
       </c>
-      <c r="B304" s="8"/>
+      <c r="B304" s="18" t="s">
+        <v>307</v>
+      </c>
       <c r="C304" s="8"/>
       <c r="D304" s="9">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="E304" s="9" t="b">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F304" s="10">
         <f t="shared" si="24"/>
@@ -46698,7 +46742,7 @@
         <v>302</v>
       </c>
       <c r="H304" s="11">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I304" s="11">
         <v>1</v>
@@ -69803,17 +69847,19 @@
     <row r="410" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A410" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B410" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="B410" s="8" t="s">
+        <v>298</v>
+      </c>
       <c r="C410" s="8"/>
       <c r="D410" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E410" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F410" s="10">
         <f t="shared" si="34"/>
@@ -69824,7 +69870,7 @@
         <v>408</v>
       </c>
       <c r="H410" s="11">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I410" s="11">
         <v>1</v>
@@ -69847,6 +69893,9 @@
       <c r="O410" t="s">
         <v>76</v>
       </c>
+      <c r="P410" t="s">
+        <v>76</v>
+      </c>
       <c r="Q410" s="12" t="s">
         <v>76</v>
       </c>
@@ -69865,7 +69914,9 @@
       <c r="V410" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W410" s="12"/>
+      <c r="W410" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X410" t="s">
         <v>76</v>
       </c>
@@ -69884,6 +69935,9 @@
       <c r="AC410" t="s">
         <v>76</v>
       </c>
+      <c r="AD410" t="s">
+        <v>76</v>
+      </c>
       <c r="AE410" s="12" t="s">
         <v>76</v>
       </c>
@@ -69902,7 +69956,9 @@
       <c r="AJ410" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK410" s="12"/>
+      <c r="AK410" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL410" t="s">
         <v>76</v>
       </c>
@@ -69921,6 +69977,9 @@
       <c r="AQ410" t="s">
         <v>76</v>
       </c>
+      <c r="AR410" t="s">
+        <v>76</v>
+      </c>
       <c r="AS410" s="12" t="s">
         <v>76</v>
       </c>
@@ -69937,127 +69996,166 @@
         <v>76</v>
       </c>
       <c r="AX410" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY410" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ410" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA410" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB410" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC410" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD410" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE410" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF410" t="s">
         <v>77</v>
       </c>
-      <c r="AY410" s="12"/>
       <c r="BG410" s="13"/>
-      <c r="BH410" s="13" t="s">
+      <c r="BH410" s="13"/>
+      <c r="BI410" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ410" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK410" s="13"/>
+      <c r="BL410" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM410" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP410" t="s">
         <v>87</v>
       </c>
-      <c r="BI410" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BJ410" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="BK410" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BL410" s="13" t="s">
+      <c r="BQ410" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR410" t="s">
+        <v>78</v>
+      </c>
+      <c r="BS410" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT410" t="s">
         <v>80</v>
       </c>
-      <c r="BM410" s="13"/>
-      <c r="BN410" t="s">
+      <c r="BU410" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV410" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BO410" t="s">
+      <c r="BW410" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="BP410" t="s">
-        <v>78</v>
-      </c>
-      <c r="BQ410" t="s">
+      <c r="BX410" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BY410" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BR410" t="s">
-        <v>79</v>
-      </c>
-      <c r="BS410" t="s">
-        <v>80</v>
-      </c>
-      <c r="BU410" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BV410" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="BW410" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BX410" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="BY410" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BZ410" s="13"/>
+      <c r="BZ410" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="CA410" s="13"/>
       <c r="CB410" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CC410" t="s">
+        <v>79</v>
+      </c>
+      <c r="CD410" t="s">
+        <v>78</v>
+      </c>
+      <c r="CE410" t="s">
+        <v>79</v>
+      </c>
+      <c r="CF410" t="s">
+        <v>78</v>
+      </c>
+      <c r="CG410" t="s">
+        <v>79</v>
+      </c>
+      <c r="CI410" s="13"/>
+      <c r="CJ410" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CK410" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="CD410" t="s">
-        <v>78</v>
-      </c>
-      <c r="CE410" t="s">
-        <v>79</v>
-      </c>
-      <c r="CF410" t="s">
-        <v>78</v>
-      </c>
-      <c r="CG410" t="s">
-        <v>78</v>
-      </c>
-      <c r="CI410" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CJ410" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CK410" s="13" t="s">
-        <v>79</v>
-      </c>
       <c r="CL410" s="13" t="s">
         <v>78</v>
       </c>
       <c r="CM410" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN410" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CO410" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CP410" t="s">
+        <v>79</v>
+      </c>
+      <c r="CQ410" t="s">
+        <v>79</v>
+      </c>
+      <c r="CR410" t="s">
+        <v>79</v>
+      </c>
+      <c r="CS410" t="s">
+        <v>79</v>
+      </c>
+      <c r="CT410" t="s">
+        <v>78</v>
+      </c>
+      <c r="CU410" t="s">
         <v>90</v>
       </c>
-      <c r="CN410" s="13"/>
-      <c r="CO410" s="13"/>
-      <c r="CP410" t="s">
+      <c r="CW410" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="CQ410" t="s">
+      <c r="CX410" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="CS410" t="s">
-        <v>78</v>
-      </c>
-      <c r="CW410" s="13"/>
-      <c r="CX410" s="13"/>
       <c r="CY410" s="13"/>
       <c r="CZ410" s="13"/>
-      <c r="DA410" s="13"/>
+      <c r="DA410" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="DB410" s="13"/>
       <c r="DC410" s="13"/>
     </row>
     <row r="411" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A411" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B411" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="B411" s="18" t="s">
+        <v>299</v>
+      </c>
       <c r="C411" s="8"/>
       <c r="D411" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E411" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F411" s="10">
         <f t="shared" si="34"/>
@@ -70068,7 +70166,7 @@
         <v>409</v>
       </c>
       <c r="H411" s="11">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I411" s="11">
         <v>1</v>
@@ -70091,6 +70189,9 @@
       <c r="O411" t="s">
         <v>76</v>
       </c>
+      <c r="P411" t="s">
+        <v>76</v>
+      </c>
       <c r="Q411" s="12" t="s">
         <v>76</v>
       </c>
@@ -70109,7 +70210,9 @@
       <c r="V411" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W411" s="12"/>
+      <c r="W411" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X411" t="s">
         <v>76</v>
       </c>
@@ -70128,6 +70231,9 @@
       <c r="AC411" t="s">
         <v>76</v>
       </c>
+      <c r="AD411" t="s">
+        <v>76</v>
+      </c>
       <c r="AE411" s="12" t="s">
         <v>76</v>
       </c>
@@ -70146,7 +70252,9 @@
       <c r="AJ411" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK411" s="12"/>
+      <c r="AK411" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL411" t="s">
         <v>76</v>
       </c>
@@ -70165,6 +70273,9 @@
       <c r="AQ411" t="s">
         <v>76</v>
       </c>
+      <c r="AR411" t="s">
+        <v>76</v>
+      </c>
       <c r="AS411" s="12" t="s">
         <v>76</v>
       </c>
@@ -70181,24 +70292,45 @@
         <v>76</v>
       </c>
       <c r="AX411" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY411" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ411" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA411" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB411" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC411" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD411" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE411" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF411" t="s">
         <v>77</v>
       </c>
-      <c r="AY411" s="12"/>
       <c r="BG411" s="13"/>
       <c r="BH411" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BI411" s="13" t="s">
-        <v>79</v>
-      </c>
+      <c r="BI411" s="13"/>
       <c r="BJ411" s="13"/>
-      <c r="BK411" s="13" t="s">
+      <c r="BK411" s="13"/>
+      <c r="BL411" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="BL411" s="13" t="s">
+      <c r="BM411" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="BM411" s="13"/>
       <c r="BN411" t="s">
         <v>87</v>
       </c>
@@ -70209,7 +70341,7 @@
         <v>79</v>
       </c>
       <c r="BU411" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="BV411" s="13" t="s">
         <v>79</v>
@@ -70220,9 +70352,7 @@
       <c r="BX411" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="BY411" s="13" t="s">
-        <v>78</v>
-      </c>
+      <c r="BY411" s="13"/>
       <c r="BZ411" s="13"/>
       <c r="CA411" s="13"/>
       <c r="CC411" t="s">
@@ -70238,7 +70368,7 @@
         <v>79</v>
       </c>
       <c r="CG411" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="CI411" s="13"/>
       <c r="CJ411" s="13"/>
@@ -70247,46 +70377,55 @@
         <v>79</v>
       </c>
       <c r="CM411" s="13" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="CN411" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="CO411" s="13"/>
-      <c r="CP411" t="s">
+      <c r="CO411" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="CT411" t="s">
+        <v>79</v>
+      </c>
+      <c r="CU411" t="s">
+        <v>78</v>
+      </c>
+      <c r="CV411" t="s">
+        <v>79</v>
+      </c>
+      <c r="CW411" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="CQ411" t="s">
+      <c r="CX411" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="CS411" t="s">
-        <v>82</v>
-      </c>
-      <c r="CT411" t="s">
-        <v>79</v>
-      </c>
-      <c r="CW411" s="13"/>
-      <c r="CX411" s="13"/>
       <c r="CY411" s="13"/>
       <c r="CZ411" s="13"/>
-      <c r="DA411" s="13"/>
-      <c r="DB411" s="13"/>
+      <c r="DA411" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="DB411" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="DC411" s="13"/>
     </row>
     <row r="412" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A412" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B412" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="B412" s="18" t="s">
+        <v>300</v>
+      </c>
       <c r="C412" s="8"/>
       <c r="D412" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E412" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F412" s="10">
         <f t="shared" si="34"/>
@@ -70297,7 +70436,7 @@
         <v>410</v>
       </c>
       <c r="H412" s="11">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I412" s="11">
         <v>1</v>
@@ -70320,6 +70459,9 @@
       <c r="O412" t="s">
         <v>76</v>
       </c>
+      <c r="P412" t="s">
+        <v>76</v>
+      </c>
       <c r="Q412" s="12" t="s">
         <v>76</v>
       </c>
@@ -70338,7 +70480,9 @@
       <c r="V412" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W412" s="12"/>
+      <c r="W412" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X412" t="s">
         <v>76</v>
       </c>
@@ -70357,6 +70501,9 @@
       <c r="AC412" t="s">
         <v>76</v>
       </c>
+      <c r="AD412" t="s">
+        <v>76</v>
+      </c>
       <c r="AE412" s="12" t="s">
         <v>76</v>
       </c>
@@ -70375,7 +70522,9 @@
       <c r="AJ412" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK412" s="12"/>
+      <c r="AK412" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL412" t="s">
         <v>76</v>
       </c>
@@ -70394,6 +70543,9 @@
       <c r="AQ412" t="s">
         <v>76</v>
       </c>
+      <c r="AR412" t="s">
+        <v>76</v>
+      </c>
       <c r="AS412" s="12" t="s">
         <v>76</v>
       </c>
@@ -70410,9 +70562,32 @@
         <v>76</v>
       </c>
       <c r="AX412" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY412" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ412" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA412" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB412" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC412" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD412" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE412" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF412" t="s">
         <v>77</v>
       </c>
-      <c r="AY412" s="12"/>
       <c r="BG412" s="13"/>
       <c r="BH412" s="13" t="s">
         <v>78</v>
@@ -70424,12 +70599,14 @@
         <v>79</v>
       </c>
       <c r="BK412" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL412" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BL412" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="BM412" s="13"/>
+      <c r="BM412" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="BN412" t="s">
         <v>78</v>
       </c>
@@ -70443,9 +70620,12 @@
         <v>79</v>
       </c>
       <c r="BR412" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="BS412" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT412" t="s">
         <v>87</v>
       </c>
       <c r="BU412" s="13" t="s">
@@ -70455,18 +70635,20 @@
         <v>79</v>
       </c>
       <c r="BW412" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX412" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BY412" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="BX412" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="BY412" s="13" t="s">
-        <v>79</v>
-      </c>
       <c r="BZ412" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="CA412" s="13"/>
+      <c r="CA412" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="CB412" t="s">
         <v>79</v>
       </c>
@@ -70480,67 +70662,92 @@
         <v>90</v>
       </c>
       <c r="CF412" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CG412" t="s">
         <v>79</v>
       </c>
+      <c r="CH412" t="s">
+        <v>79</v>
+      </c>
       <c r="CI412" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CJ412" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CK412" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="CL412" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CM412" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN412" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CO412" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CP412" t="s">
         <v>87</v>
       </c>
-      <c r="CJ412" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CK412" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CL412" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CM412" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CN412" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CO412" s="13"/>
-      <c r="CP412" t="s">
-        <v>78</v>
-      </c>
       <c r="CQ412" t="s">
+        <v>78</v>
+      </c>
+      <c r="CR412" t="s">
+        <v>79</v>
+      </c>
+      <c r="CS412" t="s">
+        <v>79</v>
+      </c>
+      <c r="CT412" t="s">
+        <v>79</v>
+      </c>
+      <c r="CU412" t="s">
+        <v>78</v>
+      </c>
+      <c r="CV412" t="s">
+        <v>78</v>
+      </c>
+      <c r="CW412" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CX412" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="CR412" t="s">
-        <v>79</v>
-      </c>
-      <c r="CS412" t="s">
-        <v>79</v>
-      </c>
-      <c r="CT412" t="s">
-        <v>78</v>
-      </c>
-      <c r="CW412" s="13"/>
-      <c r="CX412" s="13"/>
-      <c r="CY412" s="13"/>
-      <c r="CZ412" s="13"/>
-      <c r="DA412" s="13"/>
-      <c r="DB412" s="13"/>
+      <c r="CY412" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CZ412" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="DA412" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="DB412" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="DC412" s="13"/>
     </row>
     <row r="413" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A413" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B413" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="B413" s="18" t="s">
+        <v>301</v>
+      </c>
       <c r="C413" s="8"/>
       <c r="D413" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="E413" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F413" s="10">
         <f t="shared" si="34"/>
@@ -70551,7 +70758,7 @@
         <v>411</v>
       </c>
       <c r="H413" s="11">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I413" s="11">
         <v>1</v>
@@ -70574,6 +70781,9 @@
       <c r="O413" t="s">
         <v>76</v>
       </c>
+      <c r="P413" t="s">
+        <v>76</v>
+      </c>
       <c r="Q413" s="12" t="s">
         <v>76</v>
       </c>
@@ -70592,7 +70802,9 @@
       <c r="V413" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W413" s="12"/>
+      <c r="W413" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X413" t="s">
         <v>76</v>
       </c>
@@ -70611,6 +70823,9 @@
       <c r="AC413" t="s">
         <v>76</v>
       </c>
+      <c r="AD413" t="s">
+        <v>76</v>
+      </c>
       <c r="AE413" s="12" t="s">
         <v>76</v>
       </c>
@@ -70629,7 +70844,9 @@
       <c r="AJ413" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK413" s="12"/>
+      <c r="AK413" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL413" t="s">
         <v>76</v>
       </c>
@@ -70648,6 +70865,9 @@
       <c r="AQ413" t="s">
         <v>76</v>
       </c>
+      <c r="AR413" t="s">
+        <v>76</v>
+      </c>
       <c r="AS413" s="12" t="s">
         <v>76</v>
       </c>
@@ -70664,9 +70884,32 @@
         <v>76</v>
       </c>
       <c r="AX413" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY413" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ413" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA413" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB413" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC413" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD413" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE413" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF413" t="s">
         <v>77</v>
       </c>
-      <c r="AY413" s="12"/>
       <c r="BG413" s="13"/>
       <c r="BH413" s="13" t="s">
         <v>80</v>
@@ -70675,15 +70918,17 @@
         <v>79</v>
       </c>
       <c r="BJ413" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="BK413" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="BL413" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="BL413" s="13" t="s">
+      <c r="BM413" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="BM413" s="13"/>
       <c r="BN413" t="s">
         <v>80</v>
       </c>
@@ -70697,104 +70942,134 @@
         <v>79</v>
       </c>
       <c r="BR413" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS413" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT413" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU413" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV413" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BW413" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX413" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BY413" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BZ413" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CA413" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="BS413" t="s">
+      <c r="CB413" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC413" t="s">
+        <v>79</v>
+      </c>
+      <c r="CD413" t="s">
+        <v>78</v>
+      </c>
+      <c r="CE413" t="s">
+        <v>79</v>
+      </c>
+      <c r="CF413" t="s">
+        <v>78</v>
+      </c>
+      <c r="CG413" t="s">
+        <v>79</v>
+      </c>
+      <c r="CH413" t="s">
+        <v>79</v>
+      </c>
+      <c r="CI413" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="CJ413" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CK413" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CL413" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CM413" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN413" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CO413" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CP413" t="s">
+        <v>87</v>
+      </c>
+      <c r="CQ413" t="s">
+        <v>78</v>
+      </c>
+      <c r="CR413" t="s">
+        <v>79</v>
+      </c>
+      <c r="CS413" t="s">
+        <v>79</v>
+      </c>
+      <c r="CT413" t="s">
+        <v>78</v>
+      </c>
+      <c r="CU413" t="s">
+        <v>79</v>
+      </c>
+      <c r="CV413" t="s">
+        <v>78</v>
+      </c>
+      <c r="CW413" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BU413" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BV413" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="BW413" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BX413" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="BY413" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BZ413" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CA413" s="13"/>
-      <c r="CB413" t="s">
-        <v>78</v>
-      </c>
-      <c r="CC413" t="s">
-        <v>79</v>
-      </c>
-      <c r="CD413" t="s">
-        <v>78</v>
-      </c>
-      <c r="CE413" t="s">
-        <v>79</v>
-      </c>
-      <c r="CF413" t="s">
-        <v>78</v>
-      </c>
-      <c r="CG413" t="s">
-        <v>79</v>
-      </c>
-      <c r="CI413" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="CJ413" s="13" t="s">
+      <c r="CX413" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="CY413" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="CK413" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CL413" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CM413" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CN413" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CO413" s="13"/>
-      <c r="CP413" t="s">
-        <v>82</v>
-      </c>
-      <c r="CQ413" t="s">
-        <v>90</v>
-      </c>
-      <c r="CR413" t="s">
-        <v>78</v>
-      </c>
-      <c r="CS413" t="s">
-        <v>79</v>
-      </c>
-      <c r="CT413" t="s">
-        <v>78</v>
-      </c>
-      <c r="CW413" s="13"/>
-      <c r="CX413" s="13"/>
-      <c r="CY413" s="13"/>
-      <c r="CZ413" s="13"/>
-      <c r="DA413" s="13"/>
-      <c r="DB413" s="13"/>
+      <c r="CZ413" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="DA413" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="DB413" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="DC413" s="13"/>
     </row>
     <row r="414" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A414" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B414" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="B414" s="18" t="s">
+        <v>302</v>
+      </c>
       <c r="C414" s="8"/>
       <c r="D414" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E414" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F414" s="10">
         <f t="shared" si="34"/>
@@ -70805,7 +71080,7 @@
         <v>412</v>
       </c>
       <c r="H414" s="11">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I414" s="11">
         <v>1</v>
@@ -70828,6 +71103,9 @@
       <c r="O414" t="s">
         <v>76</v>
       </c>
+      <c r="P414" t="s">
+        <v>76</v>
+      </c>
       <c r="Q414" s="12" t="s">
         <v>76</v>
       </c>
@@ -70846,7 +71124,9 @@
       <c r="V414" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W414" s="12"/>
+      <c r="W414" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X414" t="s">
         <v>76</v>
       </c>
@@ -70865,6 +71145,9 @@
       <c r="AC414" t="s">
         <v>76</v>
       </c>
+      <c r="AD414" t="s">
+        <v>76</v>
+      </c>
       <c r="AE414" s="12" t="s">
         <v>76</v>
       </c>
@@ -70883,7 +71166,9 @@
       <c r="AJ414" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK414" s="12"/>
+      <c r="AK414" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL414" t="s">
         <v>76</v>
       </c>
@@ -70902,6 +71187,9 @@
       <c r="AQ414" t="s">
         <v>76</v>
       </c>
+      <c r="AR414" t="s">
+        <v>76</v>
+      </c>
       <c r="AS414" s="12" t="s">
         <v>76</v>
       </c>
@@ -70918,107 +71206,136 @@
         <v>76</v>
       </c>
       <c r="AX414" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY414" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ414" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA414" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB414" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC414" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD414" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE414" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF414" t="s">
         <v>77</v>
       </c>
-      <c r="AY414" s="12"/>
       <c r="BG414" s="13"/>
       <c r="BH414" s="13"/>
-      <c r="BI414" s="13" t="s">
+      <c r="BI414" s="13"/>
+      <c r="BJ414" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="BJ414" s="13" t="s">
-        <v>79</v>
-      </c>
       <c r="BK414" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="BL414" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BM414" s="13"/>
-      <c r="BP414" t="s">
+        <v>78</v>
+      </c>
+      <c r="BM414" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR414" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS414" t="s">
         <v>87</v>
       </c>
-      <c r="BQ414" t="s">
-        <v>79</v>
-      </c>
-      <c r="BR414" t="s">
+      <c r="BT414" t="s">
+        <v>78</v>
+      </c>
+      <c r="BU414" s="13"/>
+      <c r="BV414" s="13"/>
+      <c r="BW414" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX414" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="BS414" t="s">
-        <v>78</v>
-      </c>
-      <c r="BU414" s="13" t="s">
+      <c r="BY414" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BZ414" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CA414" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CB414" t="s">
         <v>80</v>
       </c>
-      <c r="BV414" s="13" t="s">
+      <c r="CD414" t="s">
         <v>82</v>
-      </c>
-      <c r="BW414" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="BX414" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BY414" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="BZ414" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CA414" s="13"/>
-      <c r="CB414" t="s">
-        <v>79</v>
-      </c>
-      <c r="CC414" t="s">
-        <v>79</v>
-      </c>
-      <c r="CD414" t="s">
-        <v>79</v>
       </c>
       <c r="CE414" t="s">
         <v>90</v>
       </c>
       <c r="CF414" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CI414" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CJ414" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="CK414" s="13" t="s">
         <v>79</v>
       </c>
       <c r="CL414" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CM414" s="13" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="CN414" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CO414" s="13"/>
       <c r="CP414" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CQ414" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="CR414" t="s">
         <v>79</v>
       </c>
       <c r="CT414" t="s">
-        <v>79</v>
-      </c>
-      <c r="CW414" s="13"/>
-      <c r="CX414" s="13"/>
-      <c r="CY414" s="13"/>
+        <v>78</v>
+      </c>
+      <c r="CU414" t="s">
+        <v>78</v>
+      </c>
+      <c r="CV414" t="s">
+        <v>79</v>
+      </c>
+      <c r="CW414" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CX414" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CY414" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="CZ414" s="13"/>
       <c r="DA414" s="13"/>
-      <c r="DB414" s="13"/>
+      <c r="DB414" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="DC414" s="13"/>
     </row>
     <row r="415" spans="1:107" x14ac:dyDescent="0.2">
@@ -71026,7 +71343,7 @@
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="B415" s="8"/>
+      <c r="B415" s="17"/>
       <c r="C415" s="8"/>
       <c r="D415" s="9">
         <f t="shared" si="32"/>
@@ -71270,17 +71587,19 @@
     <row r="416" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A416" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B416" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="B416" s="18" t="s">
+        <v>303</v>
+      </c>
       <c r="C416" s="8"/>
       <c r="D416" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E416" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F416" s="10">
         <f t="shared" si="34"/>
@@ -71291,7 +71610,7 @@
         <v>414</v>
       </c>
       <c r="H416" s="11">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I416" s="11">
         <v>1</v>
@@ -71312,6 +71631,9 @@
         <v>76</v>
       </c>
       <c r="O416" t="s">
+        <v>76</v>
+      </c>
+      <c r="P416" t="s">
         <v>77</v>
       </c>
       <c r="Q416" s="12" t="s">
@@ -71332,7 +71654,9 @@
       <c r="V416" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W416" s="12"/>
+      <c r="W416" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X416" t="s">
         <v>76</v>
       </c>
@@ -71351,6 +71675,9 @@
       <c r="AC416" t="s">
         <v>76</v>
       </c>
+      <c r="AD416" t="s">
+        <v>76</v>
+      </c>
       <c r="AE416" s="12" t="s">
         <v>76</v>
       </c>
@@ -71369,7 +71696,9 @@
       <c r="AJ416" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK416" s="12"/>
+      <c r="AK416" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL416" t="s">
         <v>76</v>
       </c>
@@ -71388,25 +71717,51 @@
       <c r="AQ416" t="s">
         <v>76</v>
       </c>
+      <c r="AR416" t="s">
+        <v>76</v>
+      </c>
       <c r="AS416" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT416" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU416" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV416" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AW416" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX416" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY416" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ416" t="s">
         <v>75</v>
       </c>
-      <c r="AT416" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AU416" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AV416" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AW416" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AX416" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AY416" s="12"/>
+      <c r="BA416" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB416" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC416" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD416" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE416" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF416" t="s">
+        <v>76</v>
+      </c>
       <c r="BG416" s="13" t="s">
         <v>90</v>
       </c>
@@ -71429,9 +71784,6 @@
       <c r="BP416" t="s">
         <v>79</v>
       </c>
-      <c r="BQ416" t="s">
-        <v>78</v>
-      </c>
       <c r="BR416" t="s">
         <v>79</v>
       </c>
@@ -71455,63 +71807,72 @@
       <c r="CB416" t="s">
         <v>79</v>
       </c>
-      <c r="CC416" t="s">
+      <c r="CD416" t="s">
         <v>78</v>
       </c>
       <c r="CE416" t="s">
+        <v>79</v>
+      </c>
+      <c r="CF416" t="s">
+        <v>78</v>
+      </c>
+      <c r="CH416" t="s">
+        <v>79</v>
+      </c>
+      <c r="CI416" s="13"/>
+      <c r="CJ416" s="13"/>
+      <c r="CK416" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CL416" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CM416" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="CF416" t="s">
-        <v>79</v>
-      </c>
-      <c r="CI416" s="13"/>
-      <c r="CJ416" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CK416" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CL416" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CM416" s="13" t="s">
+      <c r="CN416" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CO416" s="13"/>
+      <c r="CT416" t="s">
+        <v>79</v>
+      </c>
+      <c r="CU416" t="s">
         <v>87</v>
       </c>
-      <c r="CN416" s="13" t="s">
+      <c r="CV416" t="s">
         <v>80</v>
-      </c>
-      <c r="CO416" s="13"/>
-      <c r="CR416" t="s">
-        <v>79</v>
-      </c>
-      <c r="CT416" t="s">
-        <v>78</v>
-      </c>
-      <c r="CU416" t="s">
-        <v>90</v>
       </c>
       <c r="CW416" s="13"/>
       <c r="CX416" s="13"/>
       <c r="CY416" s="13"/>
-      <c r="CZ416" s="13"/>
+      <c r="CZ416" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="DA416" s="13"/>
-      <c r="DB416" s="13"/>
-      <c r="DC416" s="13"/>
+      <c r="DB416" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="DC416" s="13" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="417" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A417" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B417" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="B417" s="18" t="s">
+        <v>304</v>
+      </c>
       <c r="C417" s="8"/>
       <c r="D417" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E417" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F417" s="10">
         <f t="shared" si="34"/>
@@ -71522,7 +71883,7 @@
         <v>415</v>
       </c>
       <c r="H417" s="11">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I417" s="11">
         <v>1</v>
@@ -71545,6 +71906,9 @@
       <c r="O417" t="s">
         <v>76</v>
       </c>
+      <c r="P417" t="s">
+        <v>76</v>
+      </c>
       <c r="Q417" s="12" t="s">
         <v>76</v>
       </c>
@@ -71563,7 +71927,9 @@
       <c r="V417" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W417" s="12"/>
+      <c r="W417" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X417" t="s">
         <v>76</v>
       </c>
@@ -71582,6 +71948,9 @@
       <c r="AC417" t="s">
         <v>76</v>
       </c>
+      <c r="AD417" t="s">
+        <v>76</v>
+      </c>
       <c r="AE417" s="12" t="s">
         <v>76</v>
       </c>
@@ -71600,7 +71969,9 @@
       <c r="AJ417" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK417" s="12"/>
+      <c r="AK417" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL417" t="s">
         <v>76</v>
       </c>
@@ -71619,25 +71990,51 @@
       <c r="AQ417" t="s">
         <v>76</v>
       </c>
+      <c r="AR417" t="s">
+        <v>76</v>
+      </c>
       <c r="AS417" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT417" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU417" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV417" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AW417" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX417" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY417" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ417" t="s">
         <v>75</v>
       </c>
-      <c r="AT417" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AU417" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AV417" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AW417" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AX417" s="12" t="s">
+      <c r="BA417" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB417" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC417" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD417" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE417" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF417" t="s">
         <v>77</v>
       </c>
-      <c r="AY417" s="12"/>
       <c r="BG417" s="13" t="s">
         <v>78</v>
       </c>
@@ -71654,9 +72051,11 @@
         <v>79</v>
       </c>
       <c r="BL417" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM417" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BM417" s="13"/>
       <c r="BN417" t="s">
         <v>78</v>
       </c>
@@ -71670,9 +72069,12 @@
         <v>79</v>
       </c>
       <c r="BR417" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS417" t="s">
         <v>87</v>
       </c>
-      <c r="BS417" t="s">
+      <c r="BT417" t="s">
         <v>80</v>
       </c>
       <c r="BU417" s="13" t="s">
@@ -71693,7 +72095,9 @@
       <c r="BZ417" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="CA417" s="13"/>
+      <c r="CA417" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="CB417" t="s">
         <v>79</v>
       </c>
@@ -71704,58 +72108,83 @@
         <v>79</v>
       </c>
       <c r="CE417" t="s">
+        <v>79</v>
+      </c>
+      <c r="CF417" t="s">
+        <v>79</v>
+      </c>
+      <c r="CG417" t="s">
+        <v>79</v>
+      </c>
+      <c r="CH417" t="s">
+        <v>79</v>
+      </c>
+      <c r="CI417" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CJ417" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CK417" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CL417" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="CF417" t="s">
+      <c r="CM417" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="CG417" t="s">
-        <v>79</v>
-      </c>
-      <c r="CI417" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CJ417" s="13"/>
-      <c r="CK417" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="CL417" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CM417" s="13" t="s">
-        <v>79</v>
       </c>
       <c r="CN417" s="13"/>
       <c r="CO417" s="13"/>
+      <c r="CP417" t="s">
+        <v>79</v>
+      </c>
+      <c r="CQ417" t="s">
+        <v>80</v>
+      </c>
       <c r="CR417" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="CS417" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="CT417" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="CU417" t="s">
+        <v>79</v>
+      </c>
+      <c r="CV417" t="s">
+        <v>79</v>
       </c>
       <c r="CW417" s="13"/>
       <c r="CX417" s="13"/>
-      <c r="CY417" s="13"/>
-      <c r="CZ417" s="13"/>
-      <c r="DA417" s="13"/>
+      <c r="CY417" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="CZ417" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="DA417" s="13" t="s">
+        <v>80</v>
+      </c>
       <c r="DB417" s="13"/>
       <c r="DC417" s="13"/>
     </row>
     <row r="418" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A418" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B418" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="B418" s="18" t="s">
+        <v>305</v>
+      </c>
       <c r="C418" s="8"/>
       <c r="D418" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="E418" s="9" t="b">
+        <v>25</v>
+      </c>
+      <c r="E418" s="14" t="b">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
@@ -71768,7 +72197,7 @@
         <v>416</v>
       </c>
       <c r="H418" s="11">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I418" s="11">
         <v>1</v>
@@ -71791,6 +72220,9 @@
       <c r="O418" t="s">
         <v>76</v>
       </c>
+      <c r="P418" t="s">
+        <v>76</v>
+      </c>
       <c r="Q418" s="12" t="s">
         <v>76</v>
       </c>
@@ -71809,7 +72241,9 @@
       <c r="V418" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W418" s="12"/>
+      <c r="W418" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X418" t="s">
         <v>81</v>
       </c>
@@ -71828,6 +72262,9 @@
       <c r="AC418" t="s">
         <v>81</v>
       </c>
+      <c r="AD418" t="s">
+        <v>81</v>
+      </c>
       <c r="AE418" s="12" t="s">
         <v>81</v>
       </c>
@@ -71846,24 +72283,29 @@
       <c r="AJ418" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="AK418" s="12"/>
+      <c r="AK418" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="AL418" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AM418" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AN418" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AO418" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AP418" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AQ418" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="AR418" t="s">
+        <v>81</v>
       </c>
       <c r="AS418" s="12" t="s">
         <v>76</v>
@@ -71881,9 +72323,32 @@
         <v>76</v>
       </c>
       <c r="AX418" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY418" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ418" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA418" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB418" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC418" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD418" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE418" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF418" t="s">
         <v>77</v>
       </c>
-      <c r="AY418" s="12"/>
       <c r="BG418" s="13"/>
       <c r="BH418" s="13" t="s">
         <v>78</v>
@@ -71900,7 +72365,9 @@
       <c r="BL418" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="BM418" s="13"/>
+      <c r="BM418" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="BN418" t="s">
         <v>79</v>
       </c>
@@ -71913,10 +72380,10 @@
       <c r="BQ418" t="s">
         <v>87</v>
       </c>
-      <c r="BR418" t="s">
+      <c r="BS418" t="s">
         <v>80</v>
       </c>
-      <c r="BS418" t="s">
+      <c r="BT418" t="s">
         <v>79</v>
       </c>
       <c r="BU418" s="13" t="s">
@@ -71937,7 +72404,9 @@
       <c r="BZ418" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="CA418" s="13"/>
+      <c r="CA418" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="CB418" t="s">
         <v>79</v>
       </c>
@@ -71954,64 +72423,86 @@
         <v>79</v>
       </c>
       <c r="CG418" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="CH418" t="s">
+        <v>79</v>
       </c>
       <c r="CI418" s="13" t="s">
         <v>79</v>
       </c>
       <c r="CJ418" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CK418" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CL418" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CM418" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN418" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CO418" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CP418" t="s">
+        <v>79</v>
+      </c>
+      <c r="CQ418" t="s">
         <v>80</v>
       </c>
-      <c r="CK418" s="13" t="s">
+      <c r="CS418" t="s">
         <v>90</v>
       </c>
-      <c r="CL418" s="13" t="s">
+      <c r="CT418" t="s">
         <v>82</v>
       </c>
-      <c r="CM418" s="13" t="s">
+      <c r="CU418" t="s">
         <v>87</v>
       </c>
-      <c r="CN418" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CO418" s="13"/>
-      <c r="CP418" t="s">
-        <v>79</v>
-      </c>
-      <c r="CQ418" t="s">
-        <v>79</v>
-      </c>
-      <c r="CR418" t="s">
-        <v>79</v>
-      </c>
-      <c r="CS418" t="s">
-        <v>79</v>
-      </c>
-      <c r="CT418" t="s">
-        <v>78</v>
-      </c>
-      <c r="CW418" s="13"/>
-      <c r="CX418" s="13"/>
-      <c r="CY418" s="13"/>
-      <c r="CZ418" s="13"/>
-      <c r="DA418" s="13"/>
-      <c r="DB418" s="13"/>
+      <c r="CV418" t="s">
+        <v>79</v>
+      </c>
+      <c r="CW418" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CX418" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CY418" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CZ418" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="DA418" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="DB418" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="DC418" s="13"/>
     </row>
     <row r="419" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A419" s="16">
         <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B419" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="B419" s="8" t="s">
+        <v>308</v>
+      </c>
       <c r="C419" s="8"/>
       <c r="D419" s="9">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E419" s="9" t="b">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F419" s="10">
         <f t="shared" si="34"/>
@@ -72022,7 +72513,7 @@
         <v>417</v>
       </c>
       <c r="H419" s="11">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I419" s="11">
         <v>1</v>
@@ -72045,6 +72536,9 @@
       <c r="O419" t="s">
         <v>76</v>
       </c>
+      <c r="P419" t="s">
+        <v>76</v>
+      </c>
       <c r="Q419" s="12" t="s">
         <v>76</v>
       </c>
@@ -72063,7 +72557,9 @@
       <c r="V419" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="W419" s="12"/>
+      <c r="W419" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="X419" t="s">
         <v>76</v>
       </c>
@@ -72077,11 +72573,14 @@
         <v>81</v>
       </c>
       <c r="AB419" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AC419" t="s">
         <v>76</v>
       </c>
+      <c r="AD419" t="s">
+        <v>76</v>
+      </c>
       <c r="AE419" s="12" t="s">
         <v>76</v>
       </c>
@@ -72095,12 +72594,14 @@
         <v>81</v>
       </c>
       <c r="AI419" s="12" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AJ419" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AK419" s="12"/>
+      <c r="AK419" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="AL419" t="s">
         <v>76</v>
       </c>
@@ -72108,17 +72609,20 @@
         <v>76</v>
       </c>
       <c r="AN419" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AO419" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AP419" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AQ419" t="s">
         <v>76</v>
       </c>
+      <c r="AR419" t="s">
+        <v>76</v>
+      </c>
       <c r="AS419" s="12" t="s">
         <v>76</v>
       </c>
@@ -72135,9 +72639,32 @@
         <v>76</v>
       </c>
       <c r="AX419" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY419" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ419" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA419" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB419" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC419" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD419" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE419" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF419" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="AY419" s="12"/>
       <c r="BG419" s="13"/>
       <c r="BH419" s="13" t="s">
         <v>80</v>
@@ -72146,15 +72673,17 @@
         <v>79</v>
       </c>
       <c r="BJ419" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="BK419" s="13" t="s">
         <v>78</v>
       </c>
       <c r="BL419" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BM419" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="BM419" s="13"/>
       <c r="BN419" t="s">
         <v>80</v>
       </c>
@@ -72165,12 +72694,15 @@
         <v>79</v>
       </c>
       <c r="BQ419" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="BR419" t="s">
+        <v>78</v>
+      </c>
+      <c r="BS419" t="s">
         <v>90</v>
       </c>
-      <c r="BS419" t="s">
+      <c r="BT419" t="s">
         <v>78</v>
       </c>
       <c r="BU419" s="13" t="s">
@@ -72181,59 +72713,73 @@
       </c>
       <c r="BW419" s="13"/>
       <c r="BX419" s="13"/>
-      <c r="BY419" s="13" t="s">
-        <v>78</v>
-      </c>
+      <c r="BY419" s="13"/>
       <c r="BZ419" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="CA419" s="13"/>
+      <c r="CA419" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="CB419" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CC419" t="s">
-        <v>78</v>
-      </c>
-      <c r="CF419" t="s">
         <v>79</v>
       </c>
       <c r="CG419" t="s">
         <v>79</v>
       </c>
+      <c r="CH419" t="s">
+        <v>79</v>
+      </c>
       <c r="CI419" s="13" t="s">
         <v>78</v>
       </c>
       <c r="CJ419" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CK419" s="13"/>
+      <c r="CL419" s="13"/>
+      <c r="CM419" s="13"/>
+      <c r="CN419" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CO419" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CP419" t="s">
+        <v>78</v>
+      </c>
+      <c r="CQ419" t="s">
         <v>87</v>
       </c>
-      <c r="CK419" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="CL419" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="CM419" s="13" t="s">
+      <c r="CR419" t="s">
+        <v>78</v>
+      </c>
+      <c r="CS419" t="s">
+        <v>79</v>
+      </c>
+      <c r="CT419" t="s">
+        <v>79</v>
+      </c>
+      <c r="CU419" t="s">
         <v>90</v>
       </c>
-      <c r="CN419" s="13"/>
-      <c r="CO419" s="13"/>
-      <c r="CP419" t="s">
+      <c r="CW419" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="CQ419" t="s">
-        <v>78</v>
-      </c>
-      <c r="CR419" t="s">
-        <v>78</v>
-      </c>
-      <c r="CS419" t="s">
-        <v>79</v>
-      </c>
-      <c r="CW419" s="13"/>
-      <c r="CX419" s="13"/>
-      <c r="CY419" s="13"/>
-      <c r="CZ419" s="13"/>
-      <c r="DA419" s="13"/>
+      <c r="CX419" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CY419" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CZ419" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="DA419" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="DB419" s="13"/>
       <c r="DC419" s="13"/>
     </row>

</xml_diff>